<commit_message>
STU1 Technical Correction (1.0.1) stage all changes
</commit_message>
<xml_diff>
--- a/input/images/CARINforBlueButtonProfileComparison.xlsx
+++ b/input/images/CARINforBlueButtonProfileComparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/fsh/ig-data/input/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB258927-115C-D44C-AA78-8439B214CE2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F46F72-FE53-4523-A1F6-44A76C85A147}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38360" windowHeight="23560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOBProfileComparison" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Table3[#All]</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -237,9 +238,6 @@
     <t>slice: adjudicationamounttype</t>
   </si>
   <si>
-    <t>slice: inoutnetwork</t>
-  </si>
-  <si>
     <t>slice: allowedUnits</t>
   </si>
   <si>
@@ -500,13 +498,16 @@
   </si>
   <si>
     <t>profile: C4BB Organization</t>
+  </si>
+  <si>
+    <t>slice: benefitpaymentstatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1804,24 +1805,24 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25"/>
   <cols>
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="63" customWidth="1"/>
+    <col min="2" max="2" width="35.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="63" customWidth="1"/>
     <col min="4" max="4" width="32" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.1640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="31.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33" style="2" customWidth="1"/>
+    <col min="8" max="8" width="45.125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="46.5">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +1830,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>24</v>
@@ -1847,25 +1848,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1">
       <c r="A2" s="65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="45"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="49.5" thickBot="1">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
@@ -1888,25 +1889,25 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1">
       <c r="A4" s="116" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="70"/>
       <c r="F4" s="70"/>
       <c r="G4" s="70"/>
       <c r="H4" s="71"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
       <c r="A5" s="117"/>
       <c r="B5" s="22"/>
       <c r="C5" s="23"/>
@@ -1916,7 +1917,7 @@
       <c r="G5" s="67"/>
       <c r="H5" s="72"/>
     </row>
-    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="63">
       <c r="A6" s="119" t="s">
         <v>7</v>
       </c>
@@ -1926,17 +1927,17 @@
       <c r="C6" s="48"/>
       <c r="D6" s="70"/>
       <c r="E6" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="G6" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="G6" s="70" t="s">
-        <v>118</v>
-      </c>
       <c r="H6" s="71"/>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="24" customHeight="1">
       <c r="A7" s="120"/>
       <c r="B7" s="14" t="s">
         <v>7</v>
@@ -1944,17 +1945,17 @@
       <c r="C7" s="49"/>
       <c r="D7" s="73"/>
       <c r="E7" s="73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H7" s="74"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1">
       <c r="A8" s="121"/>
       <c r="B8" s="19" t="s">
         <v>8</v>
@@ -1964,13 +1965,13 @@
       </c>
       <c r="D8" s="67"/>
       <c r="E8" s="67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="67"/>
       <c r="G8" s="67"/>
       <c r="H8" s="72"/>
     </row>
-    <row r="9" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="24" thickBot="1">
       <c r="A9" s="26" t="s">
         <v>37</v>
       </c>
@@ -1979,14 +1980,14 @@
       </c>
       <c r="C9" s="51"/>
       <c r="D9" s="75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" s="76"/>
       <c r="F9" s="76"/>
       <c r="G9" s="76"/>
       <c r="H9" s="77"/>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="24" customHeight="1">
       <c r="A10" s="122" t="s">
         <v>11</v>
       </c>
@@ -1996,13 +1997,13 @@
       <c r="C10" s="48"/>
       <c r="D10" s="78"/>
       <c r="E10" s="78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="78"/>
       <c r="G10" s="78"/>
       <c r="H10" s="79"/>
     </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1">
       <c r="A11" s="123"/>
       <c r="B11" s="29" t="s">
         <v>6</v>
@@ -2010,27 +2011,27 @@
       <c r="C11" s="23"/>
       <c r="D11" s="80"/>
       <c r="E11" s="80" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="80"/>
       <c r="H11" s="81"/>
     </row>
-    <row r="12" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="24" thickBot="1">
       <c r="A12" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="31"/>
       <c r="C12" s="52"/>
       <c r="D12" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E12" s="76"/>
       <c r="F12" s="76"/>
       <c r="G12" s="76"/>
       <c r="H12" s="77"/>
     </row>
-    <row r="13" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="31.5">
       <c r="A13" s="116" t="s">
         <v>12</v>
       </c>
@@ -2039,30 +2040,30 @@
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" s="78"/>
       <c r="F13" s="78"/>
       <c r="G13" s="78"/>
       <c r="H13" s="79"/>
     </row>
-    <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1">
       <c r="A14" s="117"/>
       <c r="B14" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="67" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E14" s="80"/>
       <c r="F14" s="80"/>
       <c r="G14" s="80"/>
       <c r="H14" s="81"/>
     </row>
-    <row r="15" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="47.25">
       <c r="A15" s="124" t="s">
         <v>10</v>
       </c>
@@ -2072,26 +2073,26 @@
       <c r="C15" s="53"/>
       <c r="D15" s="70"/>
       <c r="E15" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="F15" s="70" t="s">
-        <v>119</v>
-      </c>
-      <c r="G15" s="70" t="s">
+      <c r="H15" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="H15" s="83" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" ht="48.95" customHeight="1">
       <c r="A16" s="125"/>
       <c r="B16" s="36" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="54"/>
       <c r="D16" s="84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E16" s="84" t="s">
         <v>19</v>
@@ -2106,100 +2107,100 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="63.75" thickBot="1">
       <c r="A17" s="126"/>
       <c r="B17" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" s="86"/>
       <c r="E17" s="86"/>
       <c r="F17" s="86"/>
       <c r="G17" s="86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" s="87"/>
     </row>
-    <row r="18" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A18" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="38"/>
       <c r="C18" s="56"/>
       <c r="D18" s="107" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E18" s="88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F18" s="88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G18" s="89"/>
       <c r="H18" s="90"/>
     </row>
-    <row r="19" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A19" s="109" t="s">
         <v>55</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" s="108" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E19" s="91"/>
       <c r="F19" s="91"/>
       <c r="G19" s="92"/>
       <c r="H19" s="93"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="30" customHeight="1">
       <c r="A20" s="118"/>
       <c r="B20" s="39" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="91"/>
       <c r="E20" s="91" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F20" s="91" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" s="91" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H20" s="94" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="32.1" customHeight="1">
       <c r="A21" s="118"/>
       <c r="B21" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="84"/>
       <c r="E21" s="84"/>
       <c r="F21" s="84"/>
       <c r="G21" s="84" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H21" s="85"/>
     </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A22" s="118"/>
       <c r="B22" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="84"/>
@@ -2216,7 +2217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="33.950000000000003" customHeight="1">
       <c r="A23" s="118"/>
       <c r="B23" s="36" t="s">
         <v>28</v>
@@ -2226,15 +2227,15 @@
       </c>
       <c r="D23" s="84"/>
       <c r="E23" s="84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F23" s="84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G23" s="84"/>
       <c r="H23" s="85"/>
     </row>
-    <row r="24" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="30.95" customHeight="1">
       <c r="A24" s="118"/>
       <c r="B24" s="40" t="s">
         <v>29</v>
@@ -2244,15 +2245,15 @@
       </c>
       <c r="D24" s="84"/>
       <c r="E24" s="84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" s="84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G24" s="84"/>
       <c r="H24" s="85"/>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="30" customHeight="1">
       <c r="A25" s="118"/>
       <c r="B25" s="36" t="s">
         <v>30</v>
@@ -2262,15 +2263,15 @@
       </c>
       <c r="D25" s="84"/>
       <c r="E25" s="84" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" s="84" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G25" s="84"/>
       <c r="H25" s="85"/>
     </row>
-    <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A26" s="118"/>
       <c r="B26" s="40" t="s">
         <v>31</v>
@@ -2280,31 +2281,31 @@
       </c>
       <c r="D26" s="84"/>
       <c r="E26" s="84" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F26" s="84" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26" s="84"/>
       <c r="H26" s="85"/>
     </row>
-    <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A27" s="118"/>
       <c r="B27" s="36" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="84"/>
       <c r="E27" s="84" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F27" s="84"/>
       <c r="G27" s="84"/>
       <c r="H27" s="85"/>
     </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A28" s="118"/>
       <c r="B28" s="40" t="s">
         <v>32</v>
@@ -2317,13 +2318,13 @@
       <c r="F28" s="84"/>
       <c r="G28" s="84"/>
       <c r="H28" s="85" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A29" s="118"/>
       <c r="B29" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" s="54" t="s">
         <v>22</v>
@@ -2333,13 +2334,13 @@
       <c r="F29" s="84"/>
       <c r="G29" s="84"/>
       <c r="H29" s="85" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A30" s="118"/>
       <c r="B30" s="40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" s="59"/>
       <c r="D30" s="84"/>
@@ -2350,10 +2351,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="18.95" customHeight="1">
       <c r="A31" s="118"/>
       <c r="B31" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C31" s="54" t="s">
         <v>22</v>
@@ -2363,10 +2364,10 @@
       <c r="F31" s="84"/>
       <c r="G31" s="84"/>
       <c r="H31" s="85" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="33" customHeight="1">
       <c r="A32" s="118"/>
       <c r="B32" s="40" t="s">
         <v>33</v>
@@ -2379,10 +2380,10 @@
       <c r="F32" s="84"/>
       <c r="G32" s="84"/>
       <c r="H32" s="85" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A33" s="118"/>
       <c r="B33" s="36" t="s">
         <v>34</v>
@@ -2396,35 +2397,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="17.100000000000001" customHeight="1">
       <c r="A34" s="118"/>
       <c r="B34" s="40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" s="59"/>
       <c r="D34" s="84"/>
       <c r="E34" s="84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F34" s="84"/>
       <c r="G34" s="84"/>
       <c r="H34" s="85"/>
     </row>
-    <row r="35" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="A35" s="110"/>
       <c r="B35" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="60"/>
       <c r="D35" s="86"/>
       <c r="E35" s="86"/>
       <c r="F35" s="86"/>
       <c r="G35" s="86" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H35" s="87"/>
     </row>
-    <row r="36" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
       <c r="A36" s="34" t="s">
         <v>56</v>
       </c>
@@ -2432,17 +2433,17 @@
         <v>6</v>
       </c>
       <c r="C36" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="88" t="s">
         <v>90</v>
-      </c>
-      <c r="D36" s="88" t="s">
-        <v>91</v>
       </c>
       <c r="E36" s="88"/>
       <c r="F36" s="88"/>
       <c r="G36" s="89"/>
       <c r="H36" s="90"/>
     </row>
-    <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="47.25">
       <c r="A37" s="127" t="s">
         <v>57</v>
       </c>
@@ -2452,59 +2453,59 @@
       <c r="C37" s="57"/>
       <c r="D37" s="91"/>
       <c r="E37" s="91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F37" s="91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G37" s="91" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H37" s="95" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="24" customHeight="1" thickBot="1">
       <c r="A38" s="128"/>
       <c r="B38" s="37" t="s">
-        <v>68</v>
+        <v>154</v>
       </c>
       <c r="C38" s="55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D38" s="86"/>
       <c r="E38" s="86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F38" s="86" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G38" s="86"/>
       <c r="H38" s="96" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="51.95" customHeight="1">
       <c r="A39" s="109" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D39" s="91"/>
       <c r="E39" s="91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F39" s="91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G39" s="91"/>
       <c r="H39" s="97"/>
     </row>
-    <row r="40" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="48" thickBot="1">
       <c r="A40" s="110"/>
       <c r="B40" s="37" t="s">
         <v>67</v>
@@ -2512,15 +2513,15 @@
       <c r="C40" s="55"/>
       <c r="D40" s="86"/>
       <c r="E40" s="86" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F40" s="86" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G40" s="98"/>
       <c r="H40" s="99"/>
     </row>
-    <row r="41" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" ht="24.95" customHeight="1">
       <c r="A41" s="111" t="s">
         <v>58</v>
       </c>
@@ -2532,60 +2533,60 @@
       </c>
       <c r="D41" s="91"/>
       <c r="E41" s="91" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F41" s="91" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G41" s="91"/>
       <c r="H41" s="97"/>
     </row>
-    <row r="42" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="24" customHeight="1">
       <c r="A42" s="112"/>
       <c r="B42" s="40" t="s">
         <v>15</v>
       </c>
       <c r="C42" s="59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" s="84"/>
       <c r="E42" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F42" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G42" s="84" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H42" s="85"/>
     </row>
-    <row r="43" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="36" customHeight="1">
       <c r="A43" s="112"/>
       <c r="B43" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" s="84"/>
       <c r="E43" s="84" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F43" s="84" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G43" s="84" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H43" s="85" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="24" customHeight="1">
       <c r="A44" s="112"/>
       <c r="B44" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" s="59" t="s">
         <v>21</v>
@@ -2594,11 +2595,11 @@
       <c r="E44" s="84"/>
       <c r="F44" s="84"/>
       <c r="G44" s="100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H44" s="85"/>
     </row>
-    <row r="45" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" ht="33.6" customHeight="1">
       <c r="A45" s="112"/>
       <c r="B45" s="36" t="s">
         <v>18</v>
@@ -2611,62 +2612,62 @@
       <c r="F45" s="84"/>
       <c r="G45" s="84"/>
       <c r="H45" s="85" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
       <c r="A46" s="113"/>
       <c r="B46" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="55"/>
       <c r="D46" s="86" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E46" s="98"/>
       <c r="F46" s="98"/>
       <c r="G46" s="98"/>
       <c r="H46" s="99"/>
     </row>
-    <row r="47" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="50.1" customHeight="1">
       <c r="A47" s="114" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47" s="91"/>
       <c r="E47" s="91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F47" s="91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G47" s="91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H47" s="97" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="24" customHeight="1">
       <c r="A48" s="114"/>
       <c r="B48" s="40" t="s">
-        <v>68</v>
+        <v>154</v>
       </c>
       <c r="C48" s="59"/>
       <c r="D48" s="84"/>
       <c r="E48" s="84"/>
       <c r="F48" s="84"/>
       <c r="G48" s="84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H48" s="85"/>
     </row>
-    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="47.25">
       <c r="A49" s="114"/>
       <c r="B49" s="36" t="s">
         <v>67</v>
@@ -2674,22 +2675,22 @@
       <c r="C49" s="54"/>
       <c r="D49" s="84"/>
       <c r="E49" s="84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F49" s="84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G49" s="84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H49" s="106" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="24" customHeight="1" thickBot="1">
       <c r="A50" s="115"/>
       <c r="B50" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="55"/>
       <c r="D50" s="86"/>
@@ -2704,16 +2705,16 @@
       </c>
       <c r="H50" s="87"/>
     </row>
-    <row r="51" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="32.25" thickBot="1">
       <c r="A51" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="35" t="s">
         <v>76</v>
-      </c>
-      <c r="B51" s="35" t="s">
-        <v>77</v>
       </c>
       <c r="C51" s="62"/>
       <c r="D51" s="101" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E51" s="101"/>
       <c r="F51" s="101"/>
@@ -2750,61 +2751,61 @@
       <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="56.1640625" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56.125" customWidth="1"/>
+    <col min="5" max="5" width="46.625" customWidth="1"/>
+    <col min="10" max="10" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" thickBot="1">
       <c r="A1" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21">
       <c r="A2" s="103" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21">
       <c r="A3" s="104"/>
       <c r="B3" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21">
       <c r="A4" s="104"/>
       <c r="B4" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21">
       <c r="A5" s="104"/>
       <c r="B5" s="10" t="s">
         <v>39</v>
@@ -2815,7 +2816,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21">
       <c r="A6" s="104"/>
       <c r="B6" s="10" t="s">
         <v>40</v>
@@ -2826,7 +2827,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21">
       <c r="A7" s="104"/>
       <c r="B7" s="10" t="s">
         <v>41</v>
@@ -2837,7 +2838,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21">
       <c r="A8" s="104"/>
       <c r="B8" s="10" t="s">
         <v>43</v>
@@ -2848,7 +2849,7 @@
       </c>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="21.75" thickBot="1">
       <c r="A9" s="105"/>
       <c r="B9" s="11" t="s">
         <v>37</v>
@@ -2859,38 +2860,38 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21">
       <c r="A10" s="103" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21">
       <c r="A11" s="104"/>
       <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21">
       <c r="A12" s="104"/>
       <c r="B12" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21">
       <c r="A13" s="104"/>
       <c r="B13" s="10" t="s">
         <v>48</v>
@@ -2899,27 +2900,27 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="21.75" thickBot="1">
       <c r="A14" s="105"/>
       <c r="B14" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21">
       <c r="A15" s="103" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21">
       <c r="A16" s="104"/>
       <c r="B16" s="10" t="s">
         <v>49</v>
@@ -2928,7 +2929,7 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="21">
       <c r="A17" s="104"/>
       <c r="B17" s="10" t="s">
         <v>50</v>
@@ -2937,7 +2938,7 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="21">
       <c r="A18" s="104"/>
       <c r="B18" s="10" t="s">
         <v>51</v>
@@ -2946,7 +2947,7 @@
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="21.75" thickBot="1">
       <c r="A19" s="105"/>
       <c r="B19" s="11" t="s">
         <v>52</v>
@@ -2955,58 +2956,58 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21">
       <c r="A20" s="103" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21">
       <c r="A21" s="13"/>
       <c r="B21" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="21">
       <c r="A22" s="13"/>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="D29" s="66"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to HIPPS description
</commit_message>
<xml_diff>
--- a/input/images/CARINforBlueButtonProfileComparison.xlsx
+++ b/input/images/CARINforBlueButtonProfileComparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F46F72-FE53-4523-A1F6-44A76C85A147}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA4225-A9DD-4A6D-9CAC-50288A04A1B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5595" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOBProfileComparison" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Table3[#All]</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
   <si>
     <t>Pharmacy</t>
   </si>
@@ -501,6 +500,12 @@
   </si>
   <si>
     <t>slice: benefitpaymentstatus</t>
+  </si>
+  <si>
+    <t>CPT or HCPCS Procedure Codes; HIPPS Rate Codes</t>
+  </si>
+  <si>
+    <t>CPT or HCPCS Procedure Codes; HIPPS Rate Codes; Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -1804,21 +1809,20 @@
   </sheetPr>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25"/>
   <cols>
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="2" width="35.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="63" customWidth="1"/>
-    <col min="4" max="4" width="32" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" style="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="43.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.75" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
@@ -1917,7 +1921,7 @@
       <c r="G5" s="67"/>
       <c r="H5" s="72"/>
     </row>
-    <row r="6" spans="1:11" ht="63">
+    <row r="6" spans="1:11" ht="47.25">
       <c r="A6" s="119" t="s">
         <v>7</v>
       </c>
@@ -2063,7 +2067,7 @@
       <c r="G14" s="80"/>
       <c r="H14" s="81"/>
     </row>
-    <row r="15" spans="1:11" ht="47.25">
+    <row r="15" spans="1:11" ht="31.5">
       <c r="A15" s="124" t="s">
         <v>10</v>
       </c>
@@ -2443,7 +2447,7 @@
       <c r="G36" s="89"/>
       <c r="H36" s="90"/>
     </row>
-    <row r="37" spans="1:8" ht="47.25">
+    <row r="37" spans="1:8" ht="31.5">
       <c r="A37" s="127" t="s">
         <v>57</v>
       </c>
@@ -2505,7 +2509,7 @@
       <c r="G39" s="91"/>
       <c r="H39" s="97"/>
     </row>
-    <row r="40" spans="1:8" ht="48" thickBot="1">
+    <row r="40" spans="1:8" ht="32.25" thickBot="1">
       <c r="A40" s="110"/>
       <c r="B40" s="37" t="s">
         <v>67</v>
@@ -2571,10 +2575,10 @@
       </c>
       <c r="D43" s="84"/>
       <c r="E43" s="84" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="F43" s="84" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="G43" s="84" t="s">
         <v>147</v>
@@ -2667,7 +2671,7 @@
       </c>
       <c r="H48" s="85"/>
     </row>
-    <row r="49" spans="1:8" ht="47.25">
+    <row r="49" spans="1:8" ht="31.5">
       <c r="A49" s="114"/>
       <c r="B49" s="36" t="s">
         <v>67</v>
@@ -2736,7 +2740,7 @@
     <mergeCell ref="A37:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="35" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="33" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
materials, code system, and identifier updates
</commit_message>
<xml_diff>
--- a/input/images/CARINforBlueButtonProfileComparison.xlsx
+++ b/input/images/CARINforBlueButtonProfileComparison.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EA4225-A9DD-4A6D-9CAC-50288A04A1B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBDD8249-7D47-46A1-9F9F-4F851E7F35C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5595" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOBProfileComparison" sheetId="1" r:id="rId1"/>
     <sheet name="Other Profile Comparison" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$K$51</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$H$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$H$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$H$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Table3[#All]</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="162">
   <si>
     <t>Pharmacy</t>
   </si>
@@ -181,12 +181,6 @@
   </si>
   <si>
     <t>identifier[memberid]</t>
-  </si>
-  <si>
-    <t>identifier[medrecnum]</t>
-  </si>
-  <si>
-    <t>identifier[pacctnum]</t>
   </si>
   <si>
     <t>identifier[uniquememberid]</t>
@@ -506,6 +500,27 @@
   </si>
   <si>
     <t>CPT or HCPCS Procedure Codes; HIPPS Rate Codes; Not Applicable</t>
+  </si>
+  <si>
+    <t>subType</t>
+  </si>
+  <si>
+    <t>HL7</t>
+  </si>
+  <si>
+    <t>C4BB Institutional Claim Sub Type, value = institutionalinpatient</t>
+  </si>
+  <si>
+    <t>C4BB Institutional Claim Sub Type, value = institutionaloutpatient</t>
+  </si>
+  <si>
+    <t>slice: patientaccountnumber</t>
+  </si>
+  <si>
+    <t>data in valueString</t>
+  </si>
+  <si>
+    <t>slice:medicalrecordnumber</t>
   </si>
 </sst>
 </file>
@@ -1388,9 +1403,6 @@
     <xf numFmtId="49" fontId="2" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1419,6 +1431,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1488,8 +1503,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E22" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:E22" xr:uid="{00000000-0009-0000-0100-000003000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1807,11 +1822,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:H51"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25"/>
@@ -1826,7 +1841,7 @@
     <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="46.5">
+    <row r="1" spans="1:11" s="3" customFormat="1">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1834,19 +1849,19 @@
         <v>5</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>0</v>
@@ -1854,483 +1869,488 @@
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1">
       <c r="A2" s="65" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
       <c r="H2" s="45"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="49.5" thickBot="1">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="C3" s="23" t="s">
+        <v>156</v>
+      </c>
       <c r="D3" s="67" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3" s="68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="68" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H3" s="69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1">
-      <c r="A4" s="116" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="48.6" customHeight="1" thickBot="1">
+      <c r="A4" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>158</v>
+      </c>
       <c r="G4" s="70"/>
       <c r="H4" s="71"/>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
-      <c r="A5" s="117"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="72"/>
-    </row>
-    <row r="6" spans="1:11" ht="47.25">
-      <c r="A6" s="119" t="s">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1">
+      <c r="A5" s="116" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="71"/>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
+      <c r="A6" s="117"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="72"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5">
+      <c r="A7" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B7" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70" t="s">
+      <c r="C7" s="48"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="70" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="70" t="s">
+      <c r="H7" s="71"/>
+    </row>
+    <row r="8" spans="1:11" ht="24" customHeight="1">
+      <c r="A8" s="119"/>
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="73" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="74"/>
+    </row>
+    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1">
+      <c r="A9" s="120"/>
+      <c r="B9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="72"/>
+    </row>
+    <row r="10" spans="1:11" ht="24" thickBot="1">
+      <c r="A10" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="51"/>
+      <c r="D10" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="77"/>
+    </row>
+    <row r="11" spans="1:11" ht="24" customHeight="1">
+      <c r="A11" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="79"/>
+    </row>
+    <row r="12" spans="1:11" ht="24" customHeight="1" thickBot="1">
+      <c r="A12" s="122"/>
+      <c r="B12" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="81"/>
+    </row>
+    <row r="13" spans="1:11" ht="24" thickBot="1">
+      <c r="A13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="77"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75">
+      <c r="A14" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="79"/>
+    </row>
+    <row r="15" spans="1:11" ht="24" customHeight="1" thickBot="1">
+      <c r="A15" s="117"/>
+      <c r="B15" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="81"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75">
+      <c r="A16" s="123" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="F16" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="71"/>
-    </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1">
-      <c r="A7" s="120"/>
-      <c r="B7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="H7" s="74"/>
-    </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A8" s="121"/>
-      <c r="B8" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67" t="s">
-        <v>123</v>
-      </c>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="72"/>
-    </row>
-    <row r="9" spans="1:11" ht="24" thickBot="1">
-      <c r="A9" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="75" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="77"/>
-    </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1">
-      <c r="A10" s="122" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="79"/>
-    </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A11" s="123"/>
-      <c r="B11" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="81"/>
-    </row>
-    <row r="12" spans="1:11" ht="24" thickBot="1">
-      <c r="A12" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="75" t="s">
+      <c r="H16" s="83" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="48.95" customHeight="1">
+      <c r="A17" s="124"/>
+      <c r="B17" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="54"/>
+      <c r="D17" s="84" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
-      <c r="H12" s="77"/>
-    </row>
-    <row r="13" spans="1:11" ht="31.5">
-      <c r="A13" s="116" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="70" t="s">
+      <c r="E17" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="84" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="57.75" customHeight="1" thickBot="1">
+      <c r="A18" s="125"/>
+      <c r="B18" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="87"/>
+    </row>
+    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="A19" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="88" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="89"/>
+      <c r="H19" s="90"/>
+    </row>
+    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="A20" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="108" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-    </row>
-    <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A14" s="117"/>
-      <c r="B14" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="50" t="s">
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="93"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1">
+      <c r="A21" s="128"/>
+      <c r="B21" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="91" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="94" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="32.1" customHeight="1">
+      <c r="A22" s="128"/>
+      <c r="B22" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" s="85"/>
+    </row>
+    <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A23" s="128"/>
+      <c r="B23" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="81"/>
-    </row>
-    <row r="15" spans="1:11" ht="31.5">
-      <c r="A15" s="124" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="82" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="70" t="s">
-        <v>118</v>
-      </c>
-      <c r="G15" s="70" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="83" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="48.95" customHeight="1">
-      <c r="A16" s="125"/>
-      <c r="B16" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="84" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="85" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="63.75" thickBot="1">
-      <c r="A17" s="126"/>
-      <c r="B17" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="87"/>
-    </row>
-    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A18" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="107" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="88" t="s">
-        <v>153</v>
-      </c>
-      <c r="F18" s="88" t="s">
-        <v>153</v>
-      </c>
-      <c r="G18" s="89"/>
-      <c r="H18" s="90"/>
-    </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A19" s="109" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="108" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="93"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1">
-      <c r="A20" s="118"/>
-      <c r="B20" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="91" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" s="91" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="94" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="32.1" customHeight="1">
-      <c r="A21" s="118"/>
-      <c r="B21" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="H21" s="85"/>
-    </row>
-    <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="118"/>
-      <c r="B22" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="33.950000000000003" customHeight="1">
-      <c r="A23" s="118"/>
-      <c r="B23" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="54" t="s">
-        <v>23</v>
-      </c>
+      <c r="C23" s="59"/>
       <c r="D23" s="84"/>
       <c r="E23" s="84" t="s">
-        <v>133</v>
+        <v>2</v>
       </c>
       <c r="F23" s="84" t="s">
-        <v>133</v>
-      </c>
-      <c r="G23" s="84"/>
-      <c r="H23" s="85"/>
-    </row>
-    <row r="24" spans="1:8" ht="30.95" customHeight="1">
-      <c r="A24" s="118"/>
-      <c r="B24" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="33.950000000000003" customHeight="1">
+      <c r="A24" s="128"/>
+      <c r="B24" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="54" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="84"/>
       <c r="E24" s="84" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F24" s="84" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G24" s="84"/>
       <c r="H24" s="85"/>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1">
-      <c r="A25" s="118"/>
-      <c r="B25" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="54" t="s">
+    <row r="25" spans="1:8" ht="30.95" customHeight="1">
+      <c r="A25" s="128"/>
+      <c r="B25" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="59" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="84"/>
       <c r="E25" s="84" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F25" s="84" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G25" s="84"/>
       <c r="H25" s="85"/>
     </row>
-    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="118"/>
-      <c r="B26" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="59" t="s">
+    <row r="26" spans="1:8" ht="30" customHeight="1">
+      <c r="A26" s="128"/>
+      <c r="B26" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="54" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="84"/>
       <c r="E26" s="84" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F26" s="84" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G26" s="84"/>
       <c r="H26" s="85"/>
     </row>
     <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="118"/>
-      <c r="B27" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>103</v>
+      <c r="A27" s="128"/>
+      <c r="B27" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>23</v>
       </c>
       <c r="D27" s="84"/>
       <c r="E27" s="84" t="s">
-        <v>137</v>
-      </c>
-      <c r="F27" s="84"/>
+        <v>134</v>
+      </c>
+      <c r="F27" s="84" t="s">
+        <v>134</v>
+      </c>
       <c r="G27" s="84"/>
       <c r="H27" s="85"/>
     </row>
     <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="118"/>
-      <c r="B28" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="59" t="s">
-        <v>22</v>
+      <c r="A28" s="128"/>
+      <c r="B28" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>101</v>
       </c>
       <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
+      <c r="E28" s="84" t="s">
+        <v>135</v>
+      </c>
       <c r="F28" s="84"/>
       <c r="G28" s="84"/>
-      <c r="H28" s="85" t="s">
-        <v>138</v>
-      </c>
+      <c r="H28" s="85"/>
     </row>
     <row r="29" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="118"/>
-      <c r="B29" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="54" t="s">
+      <c r="A29" s="128"/>
+      <c r="B29" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="59" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="84"/>
@@ -2338,45 +2358,45 @@
       <c r="F29" s="84"/>
       <c r="G29" s="84"/>
       <c r="H29" s="85" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="118"/>
-      <c r="B30" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="59"/>
+      <c r="A30" s="128"/>
+      <c r="B30" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>22</v>
+      </c>
       <c r="D30" s="84"/>
       <c r="E30" s="84"/>
       <c r="F30" s="84"/>
       <c r="G30" s="84"/>
       <c r="H30" s="85" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="18.95" customHeight="1">
-      <c r="A31" s="118"/>
-      <c r="B31" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="54" t="s">
-        <v>22</v>
-      </c>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A31" s="128"/>
+      <c r="B31" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="59"/>
       <c r="D31" s="84"/>
       <c r="E31" s="84"/>
       <c r="F31" s="84"/>
       <c r="G31" s="84"/>
       <c r="H31" s="85" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="33" customHeight="1">
-      <c r="A32" s="118"/>
-      <c r="B32" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18.95" customHeight="1">
+      <c r="A32" s="128"/>
+      <c r="B32" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="54" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="84"/>
@@ -2384,360 +2404,412 @@
       <c r="F32" s="84"/>
       <c r="G32" s="84"/>
       <c r="H32" s="85" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="118"/>
-      <c r="B33" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="54"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="33" customHeight="1">
+      <c r="A33" s="128"/>
+      <c r="B33" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="59" t="s">
+        <v>22</v>
+      </c>
       <c r="D33" s="84"/>
       <c r="E33" s="84"/>
       <c r="F33" s="84"/>
       <c r="G33" s="84"/>
       <c r="H33" s="85" t="s">
-        <v>3</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="118"/>
-      <c r="B34" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="59"/>
+      <c r="A34" s="128"/>
+      <c r="B34" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="54"/>
       <c r="D34" s="84"/>
-      <c r="E34" s="84" t="s">
-        <v>78</v>
-      </c>
+      <c r="E34" s="84"/>
       <c r="F34" s="84"/>
       <c r="G34" s="84"/>
-      <c r="H34" s="85"/>
-    </row>
-    <row r="35" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A35" s="110"/>
-      <c r="B35" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" s="87"/>
-    </row>
-    <row r="36" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A36" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="90"/>
-    </row>
-    <row r="37" spans="1:8" ht="31.5">
-      <c r="A37" s="127" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="43" t="s">
+      <c r="H34" s="85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A35" s="128"/>
+      <c r="B35" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91" t="s">
+      <c r="C35" s="59"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="85"/>
+    </row>
+    <row r="36" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A36" s="128"/>
+      <c r="B36" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="91" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="91" t="s">
-        <v>142</v>
-      </c>
-      <c r="H37" s="95" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="24" customHeight="1" thickBot="1">
-      <c r="A38" s="128"/>
-      <c r="B38" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="55" t="s">
-        <v>89</v>
-      </c>
+      <c r="H36" s="87"/>
+    </row>
+    <row r="37" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A37" s="128"/>
+      <c r="B37" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="59"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="84" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="85"/>
+    </row>
+    <row r="38" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A38" s="110"/>
+      <c r="B38" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="60"/>
       <c r="D38" s="86"/>
       <c r="E38" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="G38" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" s="87"/>
+    </row>
+    <row r="39" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
+      <c r="A39" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="88"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="90"/>
+    </row>
+    <row r="40" spans="1:8" ht="35.25" customHeight="1">
+      <c r="A40" s="126" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="57"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="91" t="s">
+        <v>140</v>
+      </c>
+      <c r="H40" s="95" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="24" customHeight="1" thickBot="1">
+      <c r="A41" s="127"/>
+      <c r="B41" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="86" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="86"/>
+      <c r="H41" s="96" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="51.95" customHeight="1">
+      <c r="A42" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="91"/>
+      <c r="E42" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" s="91"/>
+      <c r="H42" s="97"/>
+    </row>
+    <row r="43" spans="1:8" ht="32.25" thickBot="1">
+      <c r="A43" s="110"/>
+      <c r="B43" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="55"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43" s="86" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="98"/>
+      <c r="H43" s="99"/>
+    </row>
+    <row r="44" spans="1:8" ht="24.95" customHeight="1">
+      <c r="A44" s="111" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="91"/>
+      <c r="E44" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="F38" s="86" t="s">
+      <c r="F44" s="91" t="s">
         <v>143</v>
       </c>
-      <c r="G38" s="86"/>
-      <c r="H38" s="96" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="51.95" customHeight="1">
-      <c r="A39" s="109" t="s">
-        <v>101</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="57" t="s">
+      <c r="G44" s="91"/>
+      <c r="H44" s="97"/>
+    </row>
+    <row r="45" spans="1:8" ht="24" customHeight="1">
+      <c r="A45" s="112"/>
+      <c r="B45" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84" t="s">
+        <v>144</v>
+      </c>
+      <c r="F45" s="84" t="s">
+        <v>144</v>
+      </c>
+      <c r="G45" s="84" t="s">
+        <v>144</v>
+      </c>
+      <c r="H45" s="85"/>
+    </row>
+    <row r="46" spans="1:8" ht="36" customHeight="1">
+      <c r="A46" s="112"/>
+      <c r="B46" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="84"/>
+      <c r="E46" s="84" t="s">
+        <v>154</v>
+      </c>
+      <c r="F46" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" s="84" t="s">
+        <v>145</v>
+      </c>
+      <c r="H46" s="85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="24" customHeight="1">
+      <c r="A47" s="112"/>
+      <c r="B47" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="91"/>
-      <c r="E39" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="G39" s="91"/>
-      <c r="H39" s="97"/>
-    </row>
-    <row r="40" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A40" s="110"/>
-      <c r="B40" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86" t="s">
-        <v>142</v>
-      </c>
-      <c r="F40" s="86" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="98"/>
-      <c r="H40" s="99"/>
-    </row>
-    <row r="41" spans="1:8" ht="24.95" customHeight="1">
-      <c r="A41" s="111" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="F41" s="91" t="s">
-        <v>145</v>
-      </c>
-      <c r="G41" s="91"/>
-      <c r="H41" s="97"/>
-    </row>
-    <row r="42" spans="1:8" ht="24" customHeight="1">
-      <c r="A42" s="112"/>
-      <c r="B42" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C42" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84" t="s">
-        <v>146</v>
-      </c>
-      <c r="F42" s="84" t="s">
-        <v>146</v>
-      </c>
-      <c r="G42" s="84" t="s">
-        <v>146</v>
-      </c>
-      <c r="H42" s="85"/>
-    </row>
-    <row r="43" spans="1:8" ht="36" customHeight="1">
-      <c r="A43" s="112"/>
-      <c r="B43" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="54" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="84"/>
-      <c r="E43" s="84" t="s">
-        <v>156</v>
-      </c>
-      <c r="F43" s="84" t="s">
-        <v>155</v>
-      </c>
-      <c r="G43" s="84" t="s">
+      <c r="C47" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="100" t="s">
         <v>147</v>
       </c>
-      <c r="H43" s="85" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="24" customHeight="1">
-      <c r="A44" s="112"/>
-      <c r="B44" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
-      <c r="G44" s="100" t="s">
-        <v>149</v>
-      </c>
-      <c r="H44" s="85"/>
-    </row>
-    <row r="45" spans="1:8" ht="33.6" customHeight="1">
-      <c r="A45" s="112"/>
-      <c r="B45" s="36" t="s">
+      <c r="H47" s="85"/>
+    </row>
+    <row r="48" spans="1:8" ht="33.6" customHeight="1">
+      <c r="A48" s="112"/>
+      <c r="B48" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="54" t="s">
+      <c r="C48" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="84"/>
-      <c r="H45" s="85" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
-      <c r="A46" s="113"/>
-      <c r="B46" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="86" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="98"/>
-      <c r="F46" s="98"/>
-      <c r="G46" s="98"/>
-      <c r="H46" s="99"/>
-    </row>
-    <row r="47" spans="1:8" ht="50.1" customHeight="1">
-      <c r="A47" s="114" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="57" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="F47" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" s="91" t="s">
-        <v>92</v>
-      </c>
-      <c r="H47" s="97" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="24" customHeight="1">
-      <c r="A48" s="114"/>
-      <c r="B48" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C48" s="59"/>
       <c r="D48" s="84"/>
       <c r="E48" s="84"/>
       <c r="F48" s="84"/>
-      <c r="G48" s="84" t="s">
-        <v>88</v>
-      </c>
-      <c r="H48" s="85"/>
-    </row>
-    <row r="49" spans="1:8" ht="31.5">
-      <c r="A49" s="114"/>
-      <c r="B49" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="54"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84" t="s">
-        <v>142</v>
-      </c>
-      <c r="F49" s="84" t="s">
-        <v>142</v>
-      </c>
-      <c r="G49" s="84" t="s">
-        <v>142</v>
-      </c>
-      <c r="H49" s="106" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="24" customHeight="1" thickBot="1">
-      <c r="A50" s="115"/>
-      <c r="B50" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="55"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86" t="s">
+      <c r="G48" s="84"/>
+      <c r="H48" s="85" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
+      <c r="A49" s="113"/>
+      <c r="B49" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="55"/>
+      <c r="D49" s="86" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="98"/>
+      <c r="F49" s="98"/>
+      <c r="G49" s="98"/>
+      <c r="H49" s="99"/>
+    </row>
+    <row r="50" spans="1:8" ht="50.1" customHeight="1">
+      <c r="A50" s="114" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="91"/>
+      <c r="E50" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="G50" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="H50" s="97" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="24" customHeight="1">
+      <c r="A51" s="114"/>
+      <c r="B51" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" s="59"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="H51" s="85"/>
+    </row>
+    <row r="52" spans="1:8" ht="34.5" customHeight="1">
+      <c r="A52" s="114"/>
+      <c r="B52" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="54"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="F52" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="G52" s="84" t="s">
+        <v>140</v>
+      </c>
+      <c r="H52" s="106" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="24" customHeight="1" thickBot="1">
+      <c r="A53" s="115"/>
+      <c r="B53" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="55"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="F50" s="86" t="s">
+      <c r="F53" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="G50" s="86" t="s">
+      <c r="G53" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="H50" s="87"/>
-    </row>
-    <row r="51" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A51" s="18" t="s">
+      <c r="H53" s="87"/>
+    </row>
+    <row r="54" spans="1:8" ht="24" thickBot="1">
+      <c r="A54" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="62"/>
+      <c r="D54" s="101" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C51" s="62"/>
-      <c r="D51" s="101" t="s">
-        <v>77</v>
-      </c>
-      <c r="E51" s="101"/>
-      <c r="F51" s="101"/>
-      <c r="G51" s="101"/>
-      <c r="H51" s="102"/>
+      <c r="E54" s="101"/>
+      <c r="F54" s="101"/>
+      <c r="G54" s="101"/>
+      <c r="H54" s="102"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K51" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H54" xr:uid="{09320312-B1E4-436D-8EC0-376AEB2E9B64}"/>
   <mergeCells count="10">
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A19:A35"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A20:A38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="33" orientation="landscape" r:id="rId1"/>
@@ -2749,10 +2821,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
@@ -2767,24 +2839,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" ht="24" thickBot="1">
       <c r="A1" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="21">
       <c r="A2" s="103" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2794,7 +2866,7 @@
     <row r="3" spans="1:5" ht="21">
       <c r="A3" s="104"/>
       <c r="B3" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -2803,7 +2875,7 @@
     <row r="4" spans="1:5" ht="21">
       <c r="A4" s="104"/>
       <c r="B4" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2861,12 +2933,12 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="21">
       <c r="A10" s="103" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -2880,7 +2952,7 @@
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E11" s="10"/>
     </row>
@@ -2891,7 +2963,7 @@
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E12" s="10"/>
     </row>
@@ -2907,17 +2979,17 @@
     <row r="14" spans="1:5" ht="21.75" thickBot="1">
       <c r="A14" s="105"/>
       <c r="B14" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="21">
       <c r="A15" s="103" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -2933,86 +3005,68 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" ht="21">
-      <c r="A17" s="104"/>
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="1:5" ht="21.75" thickBot="1">
+      <c r="A17" s="105"/>
+      <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" ht="21">
-      <c r="A18" s="104"/>
-      <c r="B18" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="21.75" thickBot="1">
-      <c r="A19" s="105"/>
-      <c r="B19" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="A18" s="103" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="21">
+      <c r="A19" s="13"/>
+      <c r="B19" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="21">
-      <c r="A20" s="103" t="s">
-        <v>151</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="21">
-      <c r="A21" s="13"/>
-      <c r="B21" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" ht="21">
-      <c r="A22" s="13"/>
-      <c r="B22" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="A23" s="7"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="D29" s="66"/>
+      <c r="A24" s="7"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="D27" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
contained Organization and various changes
</commit_message>
<xml_diff>
--- a/input/images/CARINforBlueButtonProfileComparison.xlsx
+++ b/input/images/CARINforBlueButtonProfileComparison.xlsx
@@ -1,37 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBDD8249-7D47-46A1-9F9F-4F851E7F35C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4C8893-F438-1D43-AD06-6B4F717DDEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110240" yWindow="3520" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EOBProfileComparison" sheetId="1" r:id="rId1"/>
-    <sheet name="Other Profile Comparison" sheetId="3" r:id="rId2"/>
+    <sheet name="EOBProfileComparison" sheetId="4" r:id="rId1"/>
+    <sheet name="Other Profile Comparison" sheetId="5" r:id="rId2"/>
+    <sheet name="EOBProfileComparison - STU1" sheetId="1" r:id="rId3"/>
+    <sheet name="Other Profile Comparison - STU1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$H$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$H$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Table3[#All]</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$H$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EOBProfileComparison - STU1'!$A$1:$H$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$I$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'EOBProfileComparison - STU1'!$A$1:$H$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Table32[#All]</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Table3[#All]</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="179">
   <si>
     <t>Pharmacy</t>
   </si>
@@ -521,13 +536,64 @@
   </si>
   <si>
     <t>slice:medicalrecordnumber</t>
+  </si>
+  <si>
+    <t>C4BB Surface Codes</t>
+  </si>
+  <si>
+    <t>ADA</t>
+  </si>
+  <si>
+    <t>subSite</t>
+  </si>
+  <si>
+    <t>ADA Oral Body Site</t>
+  </si>
+  <si>
+    <t>bodySite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADA Universal Numbering </t>
+  </si>
+  <si>
+    <t>slice:missingtoothnumber</t>
+  </si>
+  <si>
+    <t>slice:additionalbodysite</t>
+  </si>
+  <si>
+    <t>data in code and timing</t>
+  </si>
+  <si>
+    <t>slice:prosthesis</t>
+  </si>
+  <si>
+    <t>data in code, timing and valueQuantity</t>
+  </si>
+  <si>
+    <t>slice:orthodontics</t>
+  </si>
+  <si>
+    <t>slice:patientaccountnumber</t>
+  </si>
+  <si>
+    <t>C4BB Institutional Claim Sub Type, value = vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value = oral</t>
+  </si>
+  <si>
+    <t>Oral</t>
+  </si>
+  <si>
+    <t>Professional and Nonclinician / Vision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -686,7 +752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1086,11 +1152,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1436,11 +1633,415 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1503,7 +2104,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5999D8FE-07C3-4D4E-B5A5-5AE5F13209C0}" name="Table32" displayName="Table32" ref="A1:E20" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1512,7 +2113,27 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Profile" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E8326CB1-4E2D-D342-B1F8-28964AAB5982}" name="Profile" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{9EA01000-436A-724C-B08C-750793BF4259}" name="Field"/>
+    <tableColumn id="3" xr3:uid="{B5CC308C-E5C4-634D-8DFA-4B078DA6D90C}" name="Binding Strength"/>
+    <tableColumn id="4" xr3:uid="{3C407186-3FF5-534A-8D49-4A6F4770D17B}" name="Reference or Binding"/>
+    <tableColumn id="5" xr3:uid="{0CEC2572-39D8-B347-ACC6-C1C0559C59ED}" name="Invariant"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0100-000003000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Profile" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Field"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Binding Strength"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Reference or Binding"/>
@@ -1818,30 +2439,1458 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76A9991-F60A-4F4E-BE3E-1DD8CE9115F6}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I60"/>
+  <sheetViews>
+    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24" style="6" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" style="129" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="130" customWidth="1"/>
+    <col min="4" max="9" width="27.6640625" style="129" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.3">
+      <c r="A1" s="207" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="208" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="208" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="208" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="208" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="208" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="208" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="209" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="210" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="211" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="191" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="186" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="185" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="212"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="71" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="213" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="192"/>
+      <c r="C3" s="172" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="164" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="165" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="165" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="165" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="182" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="214" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="71" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="213" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="192"/>
+      <c r="C4" s="172" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="164"/>
+      <c r="E4" s="165" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="165" t="s">
+        <v>158</v>
+      </c>
+      <c r="G4" s="165" t="s">
+        <v>175</v>
+      </c>
+      <c r="H4" s="181"/>
+      <c r="I4" s="215"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="216" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="193" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="174" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="159" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="159"/>
+      <c r="F5" s="159"/>
+      <c r="G5" s="159"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="217"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="218"/>
+      <c r="B6" s="173"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="164"/>
+      <c r="F6" s="164"/>
+      <c r="G6" s="164"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="219"/>
+    </row>
+    <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="220" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="175" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="174"/>
+      <c r="D7" s="159"/>
+      <c r="E7" s="159" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="159" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="159" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="181"/>
+      <c r="I7" s="217" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="221"/>
+      <c r="B8" s="194" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="180"/>
+      <c r="D8" s="178"/>
+      <c r="E8" s="178" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="178" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="178" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="179"/>
+      <c r="I8" s="222" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="223"/>
+      <c r="B9" s="195" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="165" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="164"/>
+      <c r="E9" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="164"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="177"/>
+      <c r="I9" s="219"/>
+    </row>
+    <row r="10" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="224" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="196" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="176"/>
+      <c r="D10" s="170" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="168"/>
+      <c r="F10" s="168"/>
+      <c r="G10" s="168"/>
+      <c r="H10" s="169"/>
+      <c r="I10" s="225"/>
+    </row>
+    <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="226" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="175" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="174"/>
+      <c r="D11" s="166"/>
+      <c r="E11" s="166" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="166"/>
+      <c r="G11" s="166"/>
+      <c r="H11" s="167"/>
+      <c r="I11" s="227"/>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="228"/>
+      <c r="B12" s="173" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="172"/>
+      <c r="D12" s="162"/>
+      <c r="E12" s="162" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="162"/>
+      <c r="G12" s="162"/>
+      <c r="H12" s="163"/>
+      <c r="I12" s="229"/>
+    </row>
+    <row r="13" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="230" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="197"/>
+      <c r="C13" s="171"/>
+      <c r="D13" s="170" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="168"/>
+      <c r="F13" s="168"/>
+      <c r="G13" s="168"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="225"/>
+    </row>
+    <row r="14" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="216" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="198" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="161"/>
+      <c r="D14" s="159" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="227"/>
+    </row>
+    <row r="15" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="218"/>
+      <c r="B15" s="195" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="165" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="164" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="162"/>
+      <c r="F15" s="162"/>
+      <c r="G15" s="162"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="229"/>
+    </row>
+    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="231" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="198" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="161"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="141" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="159" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="159" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="217" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A17" s="232"/>
+      <c r="B17" s="199" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="136"/>
+      <c r="D17" s="134" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="134" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="134" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="134" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="137" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="233" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="137" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="234"/>
+      <c r="B18" s="200" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="133" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="131"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="131"/>
+      <c r="G18" s="131" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="132"/>
+      <c r="I18" s="235" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="236" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="201"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="157" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="149" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="149" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="147"/>
+      <c r="H19" s="148"/>
+      <c r="I19" s="237"/>
+    </row>
+    <row r="20" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="238" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="202" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="141" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="156" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="154"/>
+      <c r="H20" s="155"/>
+      <c r="I20" s="239"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="240"/>
+      <c r="B21" s="203" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="153" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="139"/>
+      <c r="E21" s="139" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="139" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="139" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="152" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="241" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="240"/>
+      <c r="B22" s="199" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="136" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" s="137"/>
+      <c r="I22" s="233" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="240"/>
+      <c r="B23" s="204" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="138"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="134" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="134" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="233" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="240"/>
+      <c r="B24" s="199" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="134" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="134"/>
+      <c r="H24" s="137"/>
+      <c r="I24" s="233"/>
+    </row>
+    <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="240"/>
+      <c r="B25" s="204" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="138" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="134" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="134"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="233"/>
+    </row>
+    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="240"/>
+      <c r="B26" s="199" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="136" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="134" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="134"/>
+      <c r="H26" s="137"/>
+      <c r="I26" s="233"/>
+    </row>
+    <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="240"/>
+      <c r="B27" s="204" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="138" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" s="134" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="134"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="233"/>
+    </row>
+    <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="240"/>
+      <c r="B28" s="199" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="136" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="134"/>
+      <c r="E28" s="134" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="134"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="137"/>
+      <c r="I28" s="233"/>
+    </row>
+    <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="240"/>
+      <c r="B29" s="204" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="138" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="134"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="137" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" s="233"/>
+    </row>
+    <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="240"/>
+      <c r="B30" s="199" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="136" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="134"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="134"/>
+      <c r="G30" s="134"/>
+      <c r="H30" s="137" t="s">
+        <v>137</v>
+      </c>
+      <c r="I30" s="233"/>
+    </row>
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="240"/>
+      <c r="B31" s="204" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="138"/>
+      <c r="D31" s="134"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="134"/>
+      <c r="G31" s="134"/>
+      <c r="H31" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="233"/>
+    </row>
+    <row r="32" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="240"/>
+      <c r="B32" s="199" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="136" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="134"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="134"/>
+      <c r="G32" s="134"/>
+      <c r="H32" s="137" t="s">
+        <v>138</v>
+      </c>
+      <c r="I32" s="233"/>
+    </row>
+    <row r="33" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="240"/>
+      <c r="B33" s="204" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="138" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="134"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="134"/>
+      <c r="G33" s="134"/>
+      <c r="H33" s="137" t="s">
+        <v>139</v>
+      </c>
+      <c r="I33" s="233"/>
+    </row>
+    <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="240"/>
+      <c r="B34" s="199" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="136"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="134"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="137" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="233"/>
+    </row>
+    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="240"/>
+      <c r="B35" s="204" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="138"/>
+      <c r="D35" s="134"/>
+      <c r="E35" s="134" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="134"/>
+      <c r="G35" s="134"/>
+      <c r="H35" s="137"/>
+      <c r="I35" s="233"/>
+    </row>
+    <row r="36" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="240"/>
+      <c r="B36" s="205" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="151"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="131"/>
+      <c r="G36" s="131" t="s">
+        <v>142</v>
+      </c>
+      <c r="H36" s="132"/>
+      <c r="I36" s="235" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="240"/>
+      <c r="B37" s="204" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="138"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="137"/>
+      <c r="I37" s="233" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="240"/>
+      <c r="B38" s="205" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="151"/>
+      <c r="D38" s="131"/>
+      <c r="E38" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="F38" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="G38" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="H38" s="132"/>
+      <c r="I38" s="235" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="240"/>
+      <c r="B39" s="204" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="138"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="134"/>
+      <c r="G39" s="134"/>
+      <c r="H39" s="137"/>
+      <c r="I39" s="233" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="240"/>
+      <c r="B40" s="205" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="151"/>
+      <c r="D40" s="131"/>
+      <c r="E40" s="131"/>
+      <c r="F40" s="131"/>
+      <c r="G40" s="131" t="s">
+        <v>142</v>
+      </c>
+      <c r="H40" s="132"/>
+      <c r="I40" s="233" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="240"/>
+      <c r="B41" s="204" t="s">
+        <v>169</v>
+      </c>
+      <c r="C41" s="138" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="134"/>
+      <c r="E41" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="F41" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="G41" s="134" t="s">
+        <v>160</v>
+      </c>
+      <c r="H41" s="137"/>
+      <c r="I41" s="233" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="242"/>
+      <c r="B42" s="205" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="151" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="131"/>
+      <c r="E42" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="F42" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="G42" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="H42" s="132"/>
+      <c r="I42" s="233" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="243" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="206" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="150" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="149" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="149"/>
+      <c r="F43" s="149"/>
+      <c r="G43" s="147"/>
+      <c r="H43" s="148"/>
+      <c r="I43" s="237"/>
+    </row>
+    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="244" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="202" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="141"/>
+      <c r="D44" s="139"/>
+      <c r="E44" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="H44" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="I44" s="241" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="245"/>
+      <c r="B45" s="200" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="133" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45" s="131"/>
+      <c r="E45" s="131" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" s="131" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="131"/>
+      <c r="H45" s="145" t="s">
+        <v>141</v>
+      </c>
+      <c r="I45" s="235"/>
+    </row>
+    <row r="46" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" s="238" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="202" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="141" t="s">
+        <v>82</v>
+      </c>
+      <c r="D46" s="139"/>
+      <c r="E46" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" s="139"/>
+      <c r="H46" s="140"/>
+      <c r="I46" s="241"/>
+    </row>
+    <row r="47" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="242"/>
+      <c r="B47" s="200" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="133"/>
+      <c r="D47" s="131"/>
+      <c r="E47" s="131" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="131" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="142"/>
+      <c r="H47" s="143"/>
+      <c r="I47" s="246"/>
+    </row>
+    <row r="48" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="247" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="202" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="139"/>
+      <c r="E48" s="139" t="s">
+        <v>143</v>
+      </c>
+      <c r="F48" s="139" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="139"/>
+      <c r="H48" s="140"/>
+      <c r="I48" s="241"/>
+    </row>
+    <row r="49" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="248"/>
+      <c r="B49" s="204" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="138" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="134"/>
+      <c r="E49" s="134" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" s="134" t="s">
+        <v>144</v>
+      </c>
+      <c r="G49" s="134" t="s">
+        <v>144</v>
+      </c>
+      <c r="H49" s="137"/>
+      <c r="I49" s="233" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A50" s="248"/>
+      <c r="B50" s="199" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="136" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="134"/>
+      <c r="E50" s="134" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="134" t="s">
+        <v>153</v>
+      </c>
+      <c r="G50" s="134" t="s">
+        <v>145</v>
+      </c>
+      <c r="H50" s="137" t="s">
+        <v>109</v>
+      </c>
+      <c r="I50" s="233" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="248"/>
+      <c r="B51" s="204" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="138" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="134"/>
+      <c r="E51" s="134"/>
+      <c r="F51" s="134"/>
+      <c r="G51" s="144" t="s">
+        <v>147</v>
+      </c>
+      <c r="H51" s="137"/>
+      <c r="I51" s="249" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="248"/>
+      <c r="B52" s="199" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="136" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" s="134"/>
+      <c r="E52" s="134"/>
+      <c r="F52" s="134"/>
+      <c r="G52" s="134"/>
+      <c r="H52" s="137" t="s">
+        <v>110</v>
+      </c>
+      <c r="I52" s="233" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="248"/>
+      <c r="B53" s="204" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="138" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="134"/>
+      <c r="E53" s="134"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="144" t="s">
+        <v>147</v>
+      </c>
+      <c r="H53" s="137"/>
+      <c r="I53" s="249" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="248"/>
+      <c r="B54" s="199" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="136" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="134"/>
+      <c r="E54" s="134"/>
+      <c r="F54" s="134"/>
+      <c r="G54" s="134"/>
+      <c r="H54" s="137" t="s">
+        <v>110</v>
+      </c>
+      <c r="I54" s="233"/>
+    </row>
+    <row r="55" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="250"/>
+      <c r="B55" s="200" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="133"/>
+      <c r="D55" s="131" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="142"/>
+      <c r="F55" s="142"/>
+      <c r="G55" s="142"/>
+      <c r="H55" s="143"/>
+      <c r="I55" s="246"/>
+    </row>
+    <row r="56" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A56" s="251" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="202" t="s">
+        <v>93</v>
+      </c>
+      <c r="C56" s="141" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="139"/>
+      <c r="E56" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="F56" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="G56" s="139" t="s">
+        <v>90</v>
+      </c>
+      <c r="H56" s="140" t="s">
+        <v>146</v>
+      </c>
+      <c r="I56" s="241" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="251"/>
+      <c r="B57" s="204" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="138"/>
+      <c r="D57" s="134"/>
+      <c r="E57" s="134"/>
+      <c r="F57" s="134"/>
+      <c r="G57" s="134" t="s">
+        <v>86</v>
+      </c>
+      <c r="H57" s="137"/>
+      <c r="I57" s="233" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" s="251"/>
+      <c r="B58" s="199" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="136"/>
+      <c r="D58" s="134"/>
+      <c r="E58" s="134" t="s">
+        <v>140</v>
+      </c>
+      <c r="F58" s="134" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" s="134" t="s">
+        <v>140</v>
+      </c>
+      <c r="H58" s="135" t="s">
+        <v>140</v>
+      </c>
+      <c r="I58" s="233" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="252"/>
+      <c r="B59" s="200" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59" s="133"/>
+      <c r="D59" s="131"/>
+      <c r="E59" s="131" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="131" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="131" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="132"/>
+      <c r="I59" s="235" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A60" s="253" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="254" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="255"/>
+      <c r="D60" s="256" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="256"/>
+      <c r="F60" s="256"/>
+      <c r="G60" s="256"/>
+      <c r="H60" s="257"/>
+      <c r="I60" s="258"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="10">
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A20:A42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="22" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB69F31-6156-0E41-8A0A-2BABF00B0424}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="46.5" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="187" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="188"/>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="188"/>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="188"/>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="188"/>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="188"/>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="188"/>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="189"/>
+      <c r="B9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="187" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="188"/>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="188"/>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="188"/>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="189"/>
+      <c r="B14" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="187" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="188"/>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="189"/>
+      <c r="B17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="188"/>
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="188"/>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="190"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="66" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
     <col min="2" max="2" width="42" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="63" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="43.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="1"/>
+    <col min="7" max="7" width="59.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="25" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1867,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="65" t="s">
         <v>102</v>
       </c>
@@ -1885,7 +3934,7 @@
       <c r="G2" s="44"/>
       <c r="H2" s="45"/>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="26" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>6</v>
       </c>
@@ -1910,7 +3959,7 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="48.6" customHeight="1" thickBot="1">
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="48.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>155</v>
       </c>
@@ -1929,7 +3978,7 @@
       <c r="H4" s="71"/>
       <c r="K4" s="5"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1">
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="116" t="s">
         <v>70</v>
       </c>
@@ -1947,7 +3996,7 @@
       <c r="G5" s="70"/>
       <c r="H5" s="71"/>
     </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="117"/>
       <c r="B6" s="22"/>
       <c r="C6" s="23"/>
@@ -1957,7 +4006,7 @@
       <c r="G6" s="67"/>
       <c r="H6" s="72"/>
     </row>
-    <row r="7" spans="1:11" ht="31.5">
+    <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="118" t="s">
         <v>7</v>
       </c>
@@ -1977,7 +4026,7 @@
       </c>
       <c r="H7" s="71"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1">
+    <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="119"/>
       <c r="B8" s="14" t="s">
         <v>7</v>
@@ -1995,7 +4044,7 @@
       </c>
       <c r="H8" s="74"/>
     </row>
-    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1">
+    <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="120"/>
       <c r="B9" s="19" t="s">
         <v>8</v>
@@ -2011,7 +4060,7 @@
       <c r="G9" s="67"/>
       <c r="H9" s="72"/>
     </row>
-    <row r="10" spans="1:11" ht="24" thickBot="1">
+    <row r="10" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>37</v>
       </c>
@@ -2027,7 +4076,7 @@
       <c r="G10" s="76"/>
       <c r="H10" s="77"/>
     </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1">
+    <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="121" t="s">
         <v>11</v>
       </c>
@@ -2043,7 +4092,7 @@
       <c r="G11" s="78"/>
       <c r="H11" s="79"/>
     </row>
-    <row r="12" spans="1:11" ht="24" customHeight="1" thickBot="1">
+    <row r="12" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="122"/>
       <c r="B12" s="29" t="s">
         <v>6</v>
@@ -2057,7 +4106,7 @@
       <c r="G12" s="80"/>
       <c r="H12" s="81"/>
     </row>
-    <row r="13" spans="1:11" ht="24" thickBot="1">
+    <row r="13" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>35</v>
       </c>
@@ -2071,7 +4120,7 @@
       <c r="G13" s="76"/>
       <c r="H13" s="77"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75">
+    <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="116" t="s">
         <v>12</v>
       </c>
@@ -2087,7 +4136,7 @@
       <c r="G14" s="78"/>
       <c r="H14" s="79"/>
     </row>
-    <row r="15" spans="1:11" ht="24" customHeight="1" thickBot="1">
+    <row r="15" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="117"/>
       <c r="B15" s="19" t="s">
         <v>6</v>
@@ -2103,7 +4152,7 @@
       <c r="G15" s="80"/>
       <c r="H15" s="81"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75">
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="123" t="s">
         <v>10</v>
       </c>
@@ -2125,7 +4174,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="48.95" customHeight="1">
+    <row r="17" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="124"/>
       <c r="B17" s="36" t="s">
         <v>51</v>
@@ -2147,7 +4196,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="57.75" customHeight="1" thickBot="1">
+    <row r="18" spans="1:8" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="125"/>
       <c r="B18" s="37" t="s">
         <v>69</v>
@@ -2163,7 +4212,7 @@
       </c>
       <c r="H18" s="87"/>
     </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
+    <row r="19" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="33" t="s">
         <v>9</v>
       </c>
@@ -2181,7 +4230,7 @@
       <c r="G19" s="89"/>
       <c r="H19" s="90"/>
     </row>
-    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
+    <row r="20" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="109" t="s">
         <v>53</v>
       </c>
@@ -2199,7 +4248,7 @@
       <c r="G20" s="92"/>
       <c r="H20" s="93"/>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="128"/>
       <c r="B21" s="39" t="s">
         <v>26</v>
@@ -2221,7 +4270,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="32.1" customHeight="1">
+    <row r="22" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="128"/>
       <c r="B22" s="36" t="s">
         <v>27</v>
@@ -2237,7 +4286,7 @@
       </c>
       <c r="H22" s="85"/>
     </row>
-    <row r="23" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="128"/>
       <c r="B23" s="40" t="s">
         <v>89</v>
@@ -2257,7 +4306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="33.950000000000003" customHeight="1">
+    <row r="24" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="128"/>
       <c r="B24" s="36" t="s">
         <v>28</v>
@@ -2275,7 +4324,7 @@
       <c r="G24" s="84"/>
       <c r="H24" s="85"/>
     </row>
-    <row r="25" spans="1:8" ht="30.95" customHeight="1">
+    <row r="25" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="128"/>
       <c r="B25" s="40" t="s">
         <v>29</v>
@@ -2293,7 +4342,7 @@
       <c r="G25" s="84"/>
       <c r="H25" s="85"/>
     </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1">
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="128"/>
       <c r="B26" s="36" t="s">
         <v>30</v>
@@ -2311,7 +4360,7 @@
       <c r="G26" s="84"/>
       <c r="H26" s="85"/>
     </row>
-    <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="128"/>
       <c r="B27" s="40" t="s">
         <v>31</v>
@@ -2329,7 +4378,7 @@
       <c r="G27" s="84"/>
       <c r="H27" s="85"/>
     </row>
-    <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="128"/>
       <c r="B28" s="36" t="s">
         <v>58</v>
@@ -2345,7 +4394,7 @@
       <c r="G28" s="84"/>
       <c r="H28" s="85"/>
     </row>
-    <row r="29" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="128"/>
       <c r="B29" s="40" t="s">
         <v>32</v>
@@ -2361,7 +4410,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="128"/>
       <c r="B30" s="36" t="s">
         <v>91</v>
@@ -2377,7 +4426,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="128"/>
       <c r="B31" s="40" t="s">
         <v>92</v>
@@ -2391,7 +4440,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18.95" customHeight="1">
+    <row r="32" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="128"/>
       <c r="B32" s="36" t="s">
         <v>80</v>
@@ -2407,7 +4456,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="33" customHeight="1">
+    <row r="33" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="128"/>
       <c r="B33" s="40" t="s">
         <v>33</v>
@@ -2423,7 +4472,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="128"/>
       <c r="B34" s="36" t="s">
         <v>34</v>
@@ -2437,7 +4486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="128"/>
       <c r="B35" s="40" t="s">
         <v>67</v>
@@ -2451,7 +4500,7 @@
       <c r="G35" s="84"/>
       <c r="H35" s="85"/>
     </row>
-    <row r="36" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="36" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="128"/>
       <c r="B36" s="41" t="s">
         <v>68</v>
@@ -2465,7 +4514,7 @@
       </c>
       <c r="H36" s="87"/>
     </row>
-    <row r="37" spans="1:8" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="128"/>
       <c r="B37" s="40" t="s">
         <v>159</v>
@@ -2483,7 +4532,7 @@
       </c>
       <c r="H37" s="85"/>
     </row>
-    <row r="38" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="38" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="110"/>
       <c r="B38" s="41" t="s">
         <v>161</v>
@@ -2501,7 +4550,7 @@
       </c>
       <c r="H38" s="87"/>
     </row>
-    <row r="39" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
+    <row r="39" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="s">
         <v>54</v>
       </c>
@@ -2519,7 +4568,7 @@
       <c r="G39" s="89"/>
       <c r="H39" s="90"/>
     </row>
-    <row r="40" spans="1:8" ht="35.25" customHeight="1">
+    <row r="40" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="126" t="s">
         <v>55</v>
       </c>
@@ -2541,7 +4590,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="24" customHeight="1" thickBot="1">
+    <row r="41" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="127"/>
       <c r="B41" s="37" t="s">
         <v>152</v>
@@ -2561,7 +4610,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="51.95" customHeight="1">
+    <row r="42" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="109" t="s">
         <v>99</v>
       </c>
@@ -2581,7 +4630,7 @@
       <c r="G42" s="91"/>
       <c r="H42" s="97"/>
     </row>
-    <row r="43" spans="1:8" ht="32.25" thickBot="1">
+    <row r="43" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="110"/>
       <c r="B43" s="37" t="s">
         <v>65</v>
@@ -2597,7 +4646,7 @@
       <c r="G43" s="98"/>
       <c r="H43" s="99"/>
     </row>
-    <row r="44" spans="1:8" ht="24.95" customHeight="1">
+    <row r="44" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="111" t="s">
         <v>56</v>
       </c>
@@ -2617,7 +4666,7 @@
       <c r="G44" s="91"/>
       <c r="H44" s="97"/>
     </row>
-    <row r="45" spans="1:8" ht="24" customHeight="1">
+    <row r="45" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="112"/>
       <c r="B45" s="40" t="s">
         <v>15</v>
@@ -2637,7 +4686,7 @@
       </c>
       <c r="H45" s="85"/>
     </row>
-    <row r="46" spans="1:8" ht="36" customHeight="1">
+    <row r="46" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="112"/>
       <c r="B46" s="36" t="s">
         <v>16</v>
@@ -2659,7 +4708,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="24" customHeight="1">
+    <row r="47" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="112"/>
       <c r="B47" s="40" t="s">
         <v>84</v>
@@ -2675,7 +4724,7 @@
       </c>
       <c r="H47" s="85"/>
     </row>
-    <row r="48" spans="1:8" ht="33.6" customHeight="1">
+    <row r="48" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="112"/>
       <c r="B48" s="36" t="s">
         <v>18</v>
@@ -2691,7 +4740,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
+    <row r="49" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="113"/>
       <c r="B49" s="37" t="s">
         <v>71</v>
@@ -2705,7 +4754,7 @@
       <c r="G49" s="98"/>
       <c r="H49" s="99"/>
     </row>
-    <row r="50" spans="1:8" ht="50.1" customHeight="1">
+    <row r="50" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="114" t="s">
         <v>57</v>
       </c>
@@ -2729,7 +4778,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="24" customHeight="1">
+    <row r="51" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="114"/>
       <c r="B51" s="40" t="s">
         <v>152</v>
@@ -2743,7 +4792,7 @@
       </c>
       <c r="H51" s="85"/>
     </row>
-    <row r="52" spans="1:8" ht="34.5" customHeight="1">
+    <row r="52" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="114"/>
       <c r="B52" s="36" t="s">
         <v>65</v>
@@ -2763,7 +4812,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="24" customHeight="1" thickBot="1">
+    <row r="53" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="115"/>
       <c r="B53" s="37" t="s">
         <v>66</v>
@@ -2781,7 +4830,7 @@
       </c>
       <c r="H53" s="87"/>
     </row>
-    <row r="54" spans="1:8" ht="24" thickBot="1">
+    <row r="54" spans="1:8" ht="26" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>73</v>
       </c>
@@ -2816,7 +4865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -2827,17 +4876,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="56.125" customWidth="1"/>
-    <col min="5" max="5" width="46.625" customWidth="1"/>
-    <col min="10" max="10" width="11.375" customWidth="1"/>
+    <col min="4" max="4" width="56.1640625" customWidth="1"/>
+    <col min="5" max="5" width="46.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" thickBot="1">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>98</v>
       </c>
@@ -2854,7 +4903,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>124</v>
       </c>
@@ -2863,7 +4912,7 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="21">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="104"/>
       <c r="B3" s="10" t="s">
         <v>94</v>
@@ -2872,7 +4921,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" ht="21">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="10" t="s">
         <v>95</v>
@@ -2881,7 +4930,7 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="21">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="104"/>
       <c r="B5" s="10" t="s">
         <v>39</v>
@@ -2892,7 +4941,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="21">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="104"/>
       <c r="B6" s="10" t="s">
         <v>40</v>
@@ -2903,7 +4952,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="21">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="104"/>
       <c r="B7" s="10" t="s">
         <v>41</v>
@@ -2914,7 +4963,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="21">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="104"/>
       <c r="B8" s="10" t="s">
         <v>43</v>
@@ -2925,7 +4974,7 @@
       </c>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="21.75" thickBot="1">
+    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="105"/>
       <c r="B9" s="11" t="s">
         <v>37</v>
@@ -2936,7 +4985,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="103" t="s">
         <v>148</v>
       </c>
@@ -2945,7 +4994,7 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="21">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="104"/>
       <c r="B11" s="10" t="s">
         <v>46</v>
@@ -2956,7 +5005,7 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" ht="21">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="104"/>
       <c r="B12" s="10" t="s">
         <v>47</v>
@@ -2967,7 +5016,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" ht="21">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="104"/>
       <c r="B13" s="10" t="s">
         <v>48</v>
@@ -2976,7 +5025,7 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="21.75" thickBot="1">
+    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="105"/>
       <c r="B14" s="11" t="s">
         <v>96</v>
@@ -2987,7 +5036,7 @@
       </c>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="21">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="103" t="s">
         <v>125</v>
       </c>
@@ -2996,7 +5045,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="21">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="104"/>
       <c r="B16" s="10" t="s">
         <v>49</v>
@@ -3005,7 +5054,7 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" ht="21.75" thickBot="1">
+    <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="105"/>
       <c r="B17" s="11" t="s">
         <v>50</v>
@@ -3014,7 +5063,7 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="18" spans="1:5" ht="21">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="103" t="s">
         <v>149</v>
       </c>
@@ -3023,7 +5072,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="21">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="10" t="s">
         <v>104</v>
@@ -3034,7 +5083,7 @@
       </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" ht="21">
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" t="s">
         <v>103</v>
@@ -3045,27 +5094,27 @@
       </c>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D27" s="66"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FHIR-37726 & various material and diagram updates
</commit_message>
<xml_diff>
--- a/input/images/CARINforBlueButtonProfileComparison.xlsx
+++ b/input/images/CARINforBlueButtonProfileComparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4C8893-F438-1D43-AD06-6B4F717DDEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36B13B8C-EF9E-A848-B5C4-09ED577ACA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110240" yWindow="3520" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="-1940" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOBProfileComparison" sheetId="4" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="Other Profile Comparison - STU1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$H$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$H$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EOBProfileComparison - STU1'!$A$1:$H$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$I$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$I$61</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'EOBProfileComparison - STU1'!$A$1:$H$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Table32[#All]</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Table3[#All]</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="189">
   <si>
     <t>Pharmacy</t>
   </si>
@@ -577,9 +577,6 @@
     <t>slice:patientaccountnumber</t>
   </si>
   <si>
-    <t>C4BB Institutional Claim Sub Type, value = vision</t>
-  </si>
-  <si>
     <t xml:space="preserve"> value = oral</t>
   </si>
   <si>
@@ -587,6 +584,40 @@
   </si>
   <si>
     <t>Professional and Nonclinician / Vision</t>
+  </si>
+  <si>
+    <t>adjudication</t>
+  </si>
+  <si>
+    <t>C4BB Institutional Claim Sub Type, value = inpatient</t>
+  </si>
+  <si>
+    <t>C4BB Institutional Claim Sub Type, value = outpatient</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> value = professional or vision</t>
+  </si>
+  <si>
+    <t>slice:renderingnetworkcontractingstatus</t>
+  </si>
+  <si>
+    <t>USCoreProviderSpecialityNucc
+Invariant enforces maping Provider Taxonomy to careTeam.qualification when careTeam.role = rendering’</t>
+  </si>
+  <si>
+    <t>timingPeriod</t>
+  </si>
+  <si>
+    <t>profile: C4BB Practitioner</t>
+  </si>
+  <si>
+    <t>CPT or HCPCS Procedure Codes; Not Applicable (for vision)</t>
+  </si>
+  <si>
+    <t>slice:refillsAuthorized</t>
+  </si>
+  <si>
+    <t>slice:brandgenericindicator</t>
   </si>
 </sst>
 </file>
@@ -672,7 +703,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,8 +782,32 @@
         <bgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1153,26 +1208,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1190,20 +1225,9 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1213,25 +1237,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1239,46 +1252,30 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="2" tint="-0.499984740745262"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1287,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1573,278 +1570,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1854,146 +1589,236 @@
     <xf numFmtId="49" fontId="7" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="11" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2104,7 +1929,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5999D8FE-07C3-4D4E-B5A5-5AE5F13209C0}" name="Table32" displayName="Table32" ref="A1:E20" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5999D8FE-07C3-4D4E-B5A5-5AE5F13209C0}" name="Table32" displayName="Table32" ref="A1:E20" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2113,7 +1938,7 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E8326CB1-4E2D-D342-B1F8-28964AAB5982}" name="Profile" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E8326CB1-4E2D-D342-B1F8-28964AAB5982}" name="Profile" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{9EA01000-436A-724C-B08C-750793BF4259}" name="Field"/>
     <tableColumn id="3" xr3:uid="{B5CC308C-E5C4-634D-8DFA-4B078DA6D90C}" name="Binding Strength"/>
     <tableColumn id="4" xr3:uid="{3C407186-3FF5-534A-8D49-4A6F4770D17B}" name="Reference or Binding"/>
@@ -2124,7 +1949,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" headerRowDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:E20" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2133,7 +1958,7 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Profile" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Profile" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Field"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Binding Strength"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Reference or Binding"/>
@@ -2443,1204 +2268,1202 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I60"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="2" width="36.1640625" style="129" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="130" customWidth="1"/>
-    <col min="4" max="9" width="27.6640625" style="129" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="35" style="109" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="110" customWidth="1"/>
+    <col min="4" max="9" width="27.6640625" style="109" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.3">
-      <c r="A1" s="207" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="76" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="208" t="s">
+      <c r="B1" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="208" t="s">
+      <c r="C1" s="116" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="208" t="s">
+      <c r="D1" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="208" t="s">
+      <c r="E1" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="208" t="s">
+      <c r="F1" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="208" t="s">
+      <c r="G1" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="117" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="118" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="165" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="119" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="120" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="121" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="123"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="166" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="124"/>
+      <c r="C3" s="125" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="126" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="127" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="127" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="127" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="127" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="128" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="37" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="166" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="129"/>
+      <c r="C4" s="130" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="131"/>
+      <c r="E4" s="120" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="120" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" s="120"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="132"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="175" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="133" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="127" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="126" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="134"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="175"/>
+      <c r="B6" s="135"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="131"/>
+      <c r="I6" s="136"/>
+    </row>
+    <row r="7" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="176" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="137" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="127"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="126" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="126" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="126"/>
+      <c r="I7" s="134" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="176"/>
+      <c r="B8" s="135" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="130"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="131" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="131" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="138"/>
+      <c r="I8" s="136" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="176"/>
+      <c r="B9" s="137" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="127" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="134"/>
+    </row>
+    <row r="10" spans="1:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="167" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="135" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="130"/>
+      <c r="D10" s="131" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="139"/>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="140"/>
+    </row>
+    <row r="11" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="177" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="127"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="141" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="142"/>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="177"/>
+      <c r="B12" s="135" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="130"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="140"/>
+    </row>
+    <row r="13" spans="1:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="168" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="137"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="126" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="141"/>
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="142"/>
+    </row>
+    <row r="14" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="175" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="135" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="130"/>
+      <c r="D14" s="131" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
+      <c r="G14" s="139"/>
+      <c r="H14" s="139"/>
+      <c r="I14" s="140"/>
+    </row>
+    <row r="15" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="175"/>
+      <c r="B15" s="137" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="127" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="126" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="141"/>
+      <c r="F15" s="141"/>
+      <c r="G15" s="141"/>
+      <c r="H15" s="141"/>
+      <c r="I15" s="142"/>
+    </row>
+    <row r="16" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="178" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="135" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="130"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="143" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="131" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="131" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="136" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="178"/>
+      <c r="B17" s="144" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="145"/>
+      <c r="D17" s="146" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="146" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="146" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="146" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="146" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="147" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="178"/>
+      <c r="B18" s="148" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="149" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="150"/>
+      <c r="E18" s="150"/>
+      <c r="F18" s="150" t="s">
+        <v>183</v>
+      </c>
+      <c r="G18" s="150"/>
+      <c r="H18" s="150"/>
+      <c r="I18" s="151"/>
+    </row>
+    <row r="19" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="169" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="144"/>
+      <c r="C19" s="145"/>
+      <c r="D19" s="146" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="146" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="146" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="152"/>
+      <c r="H19" s="152"/>
+      <c r="I19" s="147" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="172" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="153" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="154" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="155" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="157"/>
+    </row>
+    <row r="21" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="172"/>
+      <c r="B21" s="158" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="145"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="141" t="s">
+        <v>184</v>
+      </c>
+      <c r="F21" s="146"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="160"/>
+    </row>
+    <row r="22" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="172"/>
+      <c r="B22" s="148" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="149"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="150" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="150" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="150" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="172"/>
+      <c r="B23" s="144" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="145" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="146"/>
+      <c r="E23" s="146" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="146" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" s="146"/>
+      <c r="H23" s="146"/>
+      <c r="I23" s="147"/>
+    </row>
+    <row r="24" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="172"/>
+      <c r="B24" s="148" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="150"/>
+      <c r="E24" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="G24" s="150"/>
+      <c r="H24" s="150"/>
+      <c r="I24" s="151"/>
+    </row>
+    <row r="25" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="172"/>
+      <c r="B25" s="144" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="145" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="146"/>
+      <c r="E25" s="146" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="146" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" s="146"/>
+      <c r="H25" s="146"/>
+      <c r="I25" s="147"/>
+    </row>
+    <row r="26" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="172"/>
+      <c r="B26" s="148" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="149" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="150"/>
+      <c r="E26" s="150" t="s">
+        <v>134</v>
+      </c>
+      <c r="F26" s="150" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" s="150"/>
+      <c r="H26" s="150"/>
+      <c r="I26" s="151"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="172"/>
+      <c r="B27" s="144" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="145" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="146"/>
+      <c r="E27" s="146" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="146"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="146"/>
+      <c r="I27" s="147"/>
+    </row>
+    <row r="28" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="172"/>
+      <c r="B28" s="148" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="149" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="150"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="150"/>
+      <c r="H28" s="150" t="s">
+        <v>136</v>
+      </c>
+      <c r="I28" s="151"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="172"/>
+      <c r="B29" s="144" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="145" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="146"/>
+      <c r="E29" s="146"/>
+      <c r="F29" s="146"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="146" t="s">
+        <v>137</v>
+      </c>
+      <c r="I29" s="147"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="172"/>
+      <c r="B30" s="153" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="154"/>
+      <c r="D30" s="150"/>
+      <c r="E30" s="150"/>
+      <c r="F30" s="150"/>
+      <c r="G30" s="150"/>
+      <c r="H30" s="150" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="151"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="172"/>
+      <c r="B31" s="161" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="162"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="146"/>
+      <c r="F31" s="146"/>
+      <c r="G31" s="146"/>
+      <c r="H31" s="146" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="147"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="172"/>
+      <c r="B32" s="153" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="154" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="150"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="150"/>
+      <c r="H32" s="150" t="s">
+        <v>138</v>
+      </c>
+      <c r="I32" s="151"/>
+    </row>
+    <row r="33" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="172"/>
+      <c r="B33" s="161" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="162" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="146"/>
+      <c r="E33" s="146"/>
+      <c r="F33" s="146"/>
+      <c r="G33" s="146"/>
+      <c r="H33" s="146" t="s">
+        <v>139</v>
+      </c>
+      <c r="I33" s="147"/>
+    </row>
+    <row r="34" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="172"/>
+      <c r="B34" s="153" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="154"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="150"/>
+      <c r="F34" s="150"/>
+      <c r="G34" s="150"/>
+      <c r="H34" s="150" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="151"/>
+    </row>
+    <row r="35" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="172"/>
+      <c r="B35" s="144" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="145"/>
+      <c r="D35" s="146"/>
+      <c r="E35" s="146"/>
+      <c r="F35" s="146"/>
+      <c r="G35" s="146" t="s">
+        <v>142</v>
+      </c>
+      <c r="H35" s="146"/>
+      <c r="I35" s="147" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="172"/>
+      <c r="B36" s="148" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="149"/>
+      <c r="D36" s="150"/>
+      <c r="E36" s="150" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="150" t="s">
+        <v>160</v>
+      </c>
+      <c r="G36" s="150" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="150"/>
+      <c r="I36" s="151" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="172"/>
+      <c r="B37" s="144" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="145"/>
+      <c r="D37" s="146"/>
+      <c r="E37" s="146" t="s">
+        <v>160</v>
+      </c>
+      <c r="F37" s="146" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="146" t="s">
+        <v>160</v>
+      </c>
+      <c r="H37" s="146"/>
+      <c r="I37" s="147" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="172"/>
+      <c r="B38" s="148" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="149"/>
+      <c r="D38" s="150"/>
+      <c r="E38" s="150"/>
+      <c r="F38" s="150"/>
+      <c r="G38" s="150"/>
+      <c r="H38" s="150"/>
+      <c r="I38" s="151" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="172"/>
+      <c r="B39" s="144" t="s">
+        <v>171</v>
+      </c>
+      <c r="C39" s="145"/>
+      <c r="D39" s="146"/>
+      <c r="E39" s="146"/>
+      <c r="F39" s="146"/>
+      <c r="G39" s="146"/>
+      <c r="H39" s="146"/>
+      <c r="I39" s="147" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="172"/>
+      <c r="B40" s="148" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="149" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" s="150"/>
+      <c r="E40" s="150"/>
+      <c r="F40" s="150"/>
+      <c r="G40" s="150"/>
+      <c r="H40" s="150"/>
+      <c r="I40" s="151" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="172"/>
+      <c r="B41" s="144" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="145" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="146"/>
+      <c r="E41" s="146"/>
+      <c r="F41" s="146"/>
+      <c r="G41" s="146"/>
+      <c r="H41" s="146"/>
+      <c r="I41" s="147" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="170" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="149" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="150" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="150"/>
+      <c r="F42" s="150"/>
+      <c r="G42" s="156"/>
+      <c r="H42" s="156"/>
+      <c r="I42" s="157"/>
+    </row>
+    <row r="43" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="171" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="144" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="145"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="H43" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43" s="147" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="172" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="209" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="210" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="211" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="191" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="186" t="s">
+      <c r="B44" s="148" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="185" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="212"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="71" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="213" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="172" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="164" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="165" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="165" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="165" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="182" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="214" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="71" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="213" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="192"/>
-      <c r="C4" s="172" t="s">
+      <c r="D44" s="150"/>
+      <c r="E44" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="H44" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="I44" s="151" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="172"/>
+      <c r="B45" s="144" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="164"/>
-      <c r="E4" s="165" t="s">
-        <v>157</v>
-      </c>
-      <c r="F4" s="165" t="s">
-        <v>158</v>
-      </c>
-      <c r="G4" s="165" t="s">
-        <v>175</v>
-      </c>
-      <c r="H4" s="181"/>
-      <c r="I4" s="215"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="216" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="193" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="174" t="s">
+      <c r="D45" s="146"/>
+      <c r="E45" s="146"/>
+      <c r="F45" s="146"/>
+      <c r="G45" s="146" t="s">
+        <v>119</v>
+      </c>
+      <c r="H45" s="146"/>
+      <c r="I45" s="147" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="172"/>
+      <c r="B46" s="148" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="159" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="159"/>
-      <c r="F5" s="159"/>
-      <c r="G5" s="159"/>
-      <c r="H5" s="181"/>
-      <c r="I5" s="217"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="218"/>
-      <c r="B6" s="173"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="164"/>
-      <c r="G6" s="164"/>
-      <c r="H6" s="177"/>
-      <c r="I6" s="219"/>
-    </row>
-    <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="220" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="175" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="174"/>
-      <c r="D7" s="159"/>
-      <c r="E7" s="159" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="159" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="159" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" s="181"/>
-      <c r="I7" s="217" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="221"/>
-      <c r="B8" s="194" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="178"/>
-      <c r="E8" s="178" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="178" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="178" t="s">
-        <v>111</v>
-      </c>
-      <c r="H8" s="179"/>
-      <c r="I8" s="222" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="223"/>
-      <c r="B9" s="195" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="165" t="s">
+      <c r="D46" s="150"/>
+      <c r="E46" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="F46" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="H46" s="150" t="s">
+        <v>141</v>
+      </c>
+      <c r="I46" s="151" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="172"/>
+      <c r="B47" s="161" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="162"/>
+      <c r="D47" s="146"/>
+      <c r="E47" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="146" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="152"/>
+      <c r="H47" s="152"/>
+      <c r="I47" s="160"/>
+    </row>
+    <row r="48" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="172"/>
+      <c r="B48" s="153" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="154" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="150"/>
+      <c r="E48" s="150" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="150" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48" s="150"/>
+      <c r="H48" s="150"/>
+      <c r="I48" s="151"/>
+    </row>
+    <row r="49" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="173" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="144" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="F9" s="164"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="177"/>
-      <c r="I9" s="219"/>
-    </row>
-    <row r="10" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="224" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="196" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="176"/>
-      <c r="D10" s="170" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="169"/>
-      <c r="I10" s="225"/>
-    </row>
-    <row r="11" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="226" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="175" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="174"/>
-      <c r="D11" s="166"/>
-      <c r="E11" s="166" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" s="166"/>
-      <c r="G11" s="166"/>
-      <c r="H11" s="167"/>
-      <c r="I11" s="227"/>
-    </row>
-    <row r="12" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="228"/>
-      <c r="B12" s="173" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="172"/>
-      <c r="D12" s="162"/>
-      <c r="E12" s="162" t="s">
-        <v>150</v>
-      </c>
-      <c r="F12" s="162"/>
-      <c r="G12" s="162"/>
-      <c r="H12" s="163"/>
-      <c r="I12" s="229"/>
-    </row>
-    <row r="13" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="230" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="197"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="170" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="168"/>
-      <c r="F13" s="168"/>
-      <c r="G13" s="168"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="225"/>
-    </row>
-    <row r="14" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="216" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="198" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="161"/>
-      <c r="D14" s="159" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="166"/>
-      <c r="F14" s="166"/>
-      <c r="G14" s="166"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="227"/>
-    </row>
-    <row r="15" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="218"/>
-      <c r="B15" s="195" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="165" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="164" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="162"/>
-      <c r="F15" s="162"/>
-      <c r="G15" s="162"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="229"/>
-    </row>
-    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A16" s="231" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="198" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="161"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="141" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="159" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="159" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16" s="160" t="s">
-        <v>118</v>
-      </c>
-      <c r="I16" s="217" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="232"/>
-      <c r="B17" s="199" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="136"/>
-      <c r="D17" s="134" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="134" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="134" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="134" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="137" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="233" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="137" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="234"/>
-      <c r="B18" s="200" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="133" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="131"/>
-      <c r="E18" s="131"/>
-      <c r="F18" s="131"/>
-      <c r="G18" s="131" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="132"/>
-      <c r="I18" s="235" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="236" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="201"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="157" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" s="149" t="s">
-        <v>151</v>
-      </c>
-      <c r="F19" s="149" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="147"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="237"/>
-    </row>
-    <row r="20" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="238" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="202" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="141" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="156" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="139"/>
-      <c r="F20" s="139"/>
-      <c r="G20" s="154"/>
-      <c r="H20" s="155"/>
-      <c r="I20" s="239"/>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="240"/>
-      <c r="B21" s="203" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="153" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="139"/>
-      <c r="E21" s="139" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="139" t="s">
-        <v>119</v>
-      </c>
-      <c r="G21" s="139" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="152" t="s">
-        <v>119</v>
-      </c>
-      <c r="I21" s="241" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="240"/>
-      <c r="B22" s="199" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="136" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="134"/>
-      <c r="E22" s="134"/>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" s="137"/>
-      <c r="I22" s="233" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="240"/>
-      <c r="B23" s="204" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="138"/>
-      <c r="D23" s="134"/>
-      <c r="E23" s="134" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="134" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="134" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="137" t="s">
-        <v>2</v>
-      </c>
-      <c r="I23" s="233" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="240"/>
-      <c r="B24" s="199" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="136" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="134"/>
-      <c r="E24" s="134" t="s">
-        <v>131</v>
-      </c>
-      <c r="F24" s="134" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="134"/>
-      <c r="H24" s="137"/>
-      <c r="I24" s="233"/>
-    </row>
-    <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="240"/>
-      <c r="B25" s="204" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="138" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" s="134" t="s">
-        <v>132</v>
-      </c>
-      <c r="G25" s="134"/>
-      <c r="H25" s="137"/>
-      <c r="I25" s="233"/>
-    </row>
-    <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="240"/>
-      <c r="B26" s="199" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="136" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="134" t="s">
-        <v>133</v>
-      </c>
-      <c r="G26" s="134"/>
-      <c r="H26" s="137"/>
-      <c r="I26" s="233"/>
-    </row>
-    <row r="27" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="240"/>
-      <c r="B27" s="204" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="138" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="134"/>
-      <c r="E27" s="134" t="s">
-        <v>134</v>
-      </c>
-      <c r="F27" s="134" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="134"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="233"/>
-    </row>
-    <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="240"/>
-      <c r="B28" s="199" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="136" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" s="134"/>
-      <c r="E28" s="134" t="s">
-        <v>135</v>
-      </c>
-      <c r="F28" s="134"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="137"/>
-      <c r="I28" s="233"/>
-    </row>
-    <row r="29" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="240"/>
-      <c r="B29" s="204" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="138" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="134"/>
-      <c r="E29" s="134"/>
-      <c r="F29" s="134"/>
-      <c r="G29" s="134"/>
-      <c r="H29" s="137" t="s">
-        <v>136</v>
-      </c>
-      <c r="I29" s="233"/>
-    </row>
-    <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="240"/>
-      <c r="B30" s="199" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="136" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="134"/>
-      <c r="E30" s="134"/>
-      <c r="F30" s="134"/>
-      <c r="G30" s="134"/>
-      <c r="H30" s="137" t="s">
-        <v>137</v>
-      </c>
-      <c r="I30" s="233"/>
-    </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="240"/>
-      <c r="B31" s="204" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="138"/>
-      <c r="D31" s="134"/>
-      <c r="E31" s="134"/>
-      <c r="F31" s="134"/>
-      <c r="G31" s="134"/>
-      <c r="H31" s="137" t="s">
-        <v>3</v>
-      </c>
-      <c r="I31" s="233"/>
-    </row>
-    <row r="32" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="240"/>
-      <c r="B32" s="199" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="136" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="134"/>
-      <c r="E32" s="134"/>
-      <c r="F32" s="134"/>
-      <c r="G32" s="134"/>
-      <c r="H32" s="137" t="s">
-        <v>138</v>
-      </c>
-      <c r="I32" s="233"/>
-    </row>
-    <row r="33" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A33" s="240"/>
-      <c r="B33" s="204" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="138" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="134"/>
-      <c r="E33" s="134"/>
-      <c r="F33" s="134"/>
-      <c r="G33" s="134"/>
-      <c r="H33" s="137" t="s">
-        <v>139</v>
-      </c>
-      <c r="I33" s="233"/>
-    </row>
-    <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="240"/>
-      <c r="B34" s="199" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="136"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="134"/>
-      <c r="G34" s="134"/>
-      <c r="H34" s="137" t="s">
-        <v>3</v>
-      </c>
-      <c r="I34" s="233"/>
-    </row>
-    <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="240"/>
-      <c r="B35" s="204" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="138"/>
-      <c r="D35" s="134"/>
-      <c r="E35" s="134" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="134"/>
-      <c r="G35" s="134"/>
-      <c r="H35" s="137"/>
-      <c r="I35" s="233"/>
-    </row>
-    <row r="36" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="240"/>
-      <c r="B36" s="205" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="151"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="131"/>
-      <c r="F36" s="131"/>
-      <c r="G36" s="131" t="s">
-        <v>142</v>
-      </c>
-      <c r="H36" s="132"/>
-      <c r="I36" s="235" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="240"/>
-      <c r="B37" s="204" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="138"/>
-      <c r="D37" s="134"/>
-      <c r="E37" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="F37" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="G37" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="H37" s="137"/>
-      <c r="I37" s="233" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="240"/>
-      <c r="B38" s="205" t="s">
-        <v>161</v>
-      </c>
-      <c r="C38" s="151"/>
-      <c r="D38" s="131"/>
-      <c r="E38" s="131" t="s">
-        <v>160</v>
-      </c>
-      <c r="F38" s="131" t="s">
-        <v>160</v>
-      </c>
-      <c r="G38" s="131" t="s">
-        <v>160</v>
-      </c>
-      <c r="H38" s="132"/>
-      <c r="I38" s="235" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="240"/>
-      <c r="B39" s="204" t="s">
-        <v>173</v>
-      </c>
-      <c r="C39" s="138"/>
-      <c r="D39" s="134"/>
-      <c r="E39" s="134" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="134"/>
-      <c r="G39" s="134"/>
-      <c r="H39" s="137"/>
-      <c r="I39" s="233" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="240"/>
-      <c r="B40" s="205" t="s">
-        <v>171</v>
-      </c>
-      <c r="C40" s="151"/>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="131" t="s">
-        <v>142</v>
-      </c>
-      <c r="H40" s="132"/>
-      <c r="I40" s="233" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="240"/>
-      <c r="B41" s="204" t="s">
-        <v>169</v>
-      </c>
-      <c r="C41" s="138" t="s">
+      <c r="D49" s="146"/>
+      <c r="E49" s="146" t="s">
+        <v>143</v>
+      </c>
+      <c r="F49" s="146" t="s">
+        <v>143</v>
+      </c>
+      <c r="G49" s="146"/>
+      <c r="H49" s="146"/>
+      <c r="I49" s="147"/>
+    </row>
+    <row r="50" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="173"/>
+      <c r="B50" s="148" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="149" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="150"/>
+      <c r="E50" s="150" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" s="150" t="s">
+        <v>144</v>
+      </c>
+      <c r="G50" s="150" t="s">
+        <v>144</v>
+      </c>
+      <c r="H50" s="150"/>
+      <c r="I50" s="151" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="173"/>
+      <c r="B51" s="144" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="145" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="146"/>
+      <c r="E51" s="146" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" s="146" t="s">
+        <v>154</v>
+      </c>
+      <c r="G51" s="146" t="s">
+        <v>186</v>
+      </c>
+      <c r="H51" s="146" t="s">
+        <v>109</v>
+      </c>
+      <c r="I51" s="147" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="173"/>
+      <c r="B52" s="148" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="149" t="s">
         <v>163</v>
       </c>
-      <c r="D41" s="134"/>
-      <c r="E41" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="F41" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="G41" s="134" t="s">
-        <v>160</v>
-      </c>
-      <c r="H41" s="137"/>
-      <c r="I41" s="233" t="s">
+      <c r="D52" s="150"/>
+      <c r="E52" s="150"/>
+      <c r="F52" s="150"/>
+      <c r="G52" s="163" t="s">
+        <v>147</v>
+      </c>
+      <c r="H52" s="150"/>
+      <c r="I52" s="164" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="242"/>
-      <c r="B42" s="205" t="s">
-        <v>168</v>
-      </c>
-      <c r="C42" s="151" t="s">
+    <row r="53" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="173"/>
+      <c r="B53" s="144" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" s="145" t="s">
         <v>163</v>
       </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="131" t="s">
-        <v>160</v>
-      </c>
-      <c r="F42" s="131" t="s">
-        <v>160</v>
-      </c>
-      <c r="G42" s="131" t="s">
-        <v>160</v>
-      </c>
-      <c r="H42" s="132"/>
-      <c r="I42" s="233" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="243" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="206" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="150" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" s="149" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" s="149"/>
-      <c r="F43" s="149"/>
-      <c r="G43" s="147"/>
-      <c r="H43" s="148"/>
-      <c r="I43" s="237"/>
-    </row>
-    <row r="44" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A44" s="244" t="s">
-        <v>55</v>
-      </c>
-      <c r="B44" s="202" t="s">
+      <c r="D53" s="146"/>
+      <c r="E53" s="146"/>
+      <c r="F53" s="146"/>
+      <c r="G53" s="146"/>
+      <c r="H53" s="146"/>
+      <c r="I53" s="147" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="173"/>
+      <c r="B54" s="148" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="149" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="150"/>
+      <c r="E54" s="150"/>
+      <c r="F54" s="150"/>
+      <c r="G54" s="163" t="s">
+        <v>147</v>
+      </c>
+      <c r="H54" s="150"/>
+      <c r="I54" s="164" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="173"/>
+      <c r="B55" s="144" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="145" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="146"/>
+      <c r="E55" s="146"/>
+      <c r="F55" s="146"/>
+      <c r="G55" s="146"/>
+      <c r="H55" s="146" t="s">
+        <v>110</v>
+      </c>
+      <c r="I55" s="147"/>
+    </row>
+    <row r="56" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="173"/>
+      <c r="B56" s="148" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="149"/>
+      <c r="D56" s="150" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56" s="156"/>
+      <c r="F56" s="156"/>
+      <c r="G56" s="156"/>
+      <c r="H56" s="156"/>
+      <c r="I56" s="157"/>
+    </row>
+    <row r="57" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="174" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="144" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" s="145" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="146"/>
+      <c r="E57" s="146" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="146" t="s">
+        <v>90</v>
+      </c>
+      <c r="G57" s="146" t="s">
+        <v>90</v>
+      </c>
+      <c r="H57" s="146" t="s">
+        <v>146</v>
+      </c>
+      <c r="I57" s="147" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="174"/>
+      <c r="B58" s="148" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58" s="149"/>
+      <c r="D58" s="150"/>
+      <c r="E58" s="150"/>
+      <c r="F58" s="150"/>
+      <c r="G58" s="150" t="s">
+        <v>86</v>
+      </c>
+      <c r="H58" s="150"/>
+      <c r="I58" s="151" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="174"/>
+      <c r="B59" s="144" t="s">
         <v>65</v>
       </c>
-      <c r="C44" s="141"/>
-      <c r="D44" s="139"/>
-      <c r="E44" s="139" t="s">
+      <c r="C59" s="145"/>
+      <c r="D59" s="146"/>
+      <c r="E59" s="146" t="s">
         <v>140</v>
       </c>
-      <c r="F44" s="139" t="s">
+      <c r="F59" s="146" t="s">
         <v>140</v>
       </c>
-      <c r="G44" s="139" t="s">
+      <c r="G59" s="146" t="s">
         <v>140</v>
       </c>
-      <c r="H44" s="146" t="s">
+      <c r="H59" s="146" t="s">
         <v>140</v>
       </c>
-      <c r="I44" s="241" t="s">
+      <c r="I59" s="147" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="245"/>
-      <c r="B45" s="200" t="s">
-        <v>152</v>
-      </c>
-      <c r="C45" s="133" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="131"/>
-      <c r="E45" s="131" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" s="131" t="s">
-        <v>141</v>
-      </c>
-      <c r="G45" s="131"/>
-      <c r="H45" s="145" t="s">
-        <v>141</v>
-      </c>
-      <c r="I45" s="235"/>
-    </row>
-    <row r="46" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A46" s="238" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="202" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="141" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="139"/>
-      <c r="E46" s="139" t="s">
-        <v>90</v>
-      </c>
-      <c r="F46" s="139" t="s">
-        <v>90</v>
-      </c>
-      <c r="G46" s="139"/>
-      <c r="H46" s="140"/>
-      <c r="I46" s="241"/>
-    </row>
-    <row r="47" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="242"/>
-      <c r="B47" s="200" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="133"/>
-      <c r="D47" s="131"/>
-      <c r="E47" s="131" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" s="131" t="s">
-        <v>140</v>
-      </c>
-      <c r="G47" s="142"/>
-      <c r="H47" s="143"/>
-      <c r="I47" s="246"/>
-    </row>
-    <row r="48" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="247" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="202" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="141" t="s">
-        <v>23</v>
-      </c>
-      <c r="D48" s="139"/>
-      <c r="E48" s="139" t="s">
-        <v>143</v>
-      </c>
-      <c r="F48" s="139" t="s">
-        <v>143</v>
-      </c>
-      <c r="G48" s="139"/>
-      <c r="H48" s="140"/>
-      <c r="I48" s="241"/>
-    </row>
-    <row r="49" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A49" s="248"/>
-      <c r="B49" s="204" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="138" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="134"/>
-      <c r="E49" s="134" t="s">
-        <v>144</v>
-      </c>
-      <c r="F49" s="134" t="s">
-        <v>144</v>
-      </c>
-      <c r="G49" s="134" t="s">
-        <v>144</v>
-      </c>
-      <c r="H49" s="137"/>
-      <c r="I49" s="233" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A50" s="248"/>
-      <c r="B50" s="199" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="136" t="s">
-        <v>83</v>
-      </c>
-      <c r="D50" s="134"/>
-      <c r="E50" s="134" t="s">
-        <v>154</v>
-      </c>
-      <c r="F50" s="134" t="s">
-        <v>153</v>
-      </c>
-      <c r="G50" s="134" t="s">
-        <v>145</v>
-      </c>
-      <c r="H50" s="137" t="s">
-        <v>109</v>
-      </c>
-      <c r="I50" s="233" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="248"/>
-      <c r="B51" s="204" t="s">
-        <v>166</v>
-      </c>
-      <c r="C51" s="138" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" s="134"/>
-      <c r="E51" s="134"/>
-      <c r="F51" s="134"/>
-      <c r="G51" s="144" t="s">
-        <v>147</v>
-      </c>
-      <c r="H51" s="137"/>
-      <c r="I51" s="249" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="248"/>
-      <c r="B52" s="199" t="s">
-        <v>164</v>
-      </c>
-      <c r="C52" s="136" t="s">
-        <v>163</v>
-      </c>
-      <c r="D52" s="134"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="134"/>
-      <c r="G52" s="134"/>
-      <c r="H52" s="137" t="s">
-        <v>110</v>
-      </c>
-      <c r="I52" s="233" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="248"/>
-      <c r="B53" s="204" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="138" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="134"/>
-      <c r="E53" s="134"/>
-      <c r="F53" s="134"/>
-      <c r="G53" s="144" t="s">
-        <v>147</v>
-      </c>
-      <c r="H53" s="137"/>
-      <c r="I53" s="249" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="248"/>
-      <c r="B54" s="199" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" s="136" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="134"/>
-      <c r="E54" s="134"/>
-      <c r="F54" s="134"/>
-      <c r="G54" s="134"/>
-      <c r="H54" s="137" t="s">
-        <v>110</v>
-      </c>
-      <c r="I54" s="233"/>
-    </row>
-    <row r="55" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="250"/>
-      <c r="B55" s="200" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="133"/>
-      <c r="D55" s="131" t="s">
-        <v>72</v>
-      </c>
-      <c r="E55" s="142"/>
-      <c r="F55" s="142"/>
-      <c r="G55" s="142"/>
-      <c r="H55" s="143"/>
-      <c r="I55" s="246"/>
-    </row>
-    <row r="56" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A56" s="251" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="202" t="s">
-        <v>93</v>
-      </c>
-      <c r="C56" s="141" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="139"/>
-      <c r="E56" s="139" t="s">
-        <v>90</v>
-      </c>
-      <c r="F56" s="139" t="s">
-        <v>90</v>
-      </c>
-      <c r="G56" s="139" t="s">
-        <v>90</v>
-      </c>
-      <c r="H56" s="140" t="s">
-        <v>146</v>
-      </c>
-      <c r="I56" s="241" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="251"/>
-      <c r="B57" s="204" t="s">
-        <v>152</v>
-      </c>
-      <c r="C57" s="138"/>
-      <c r="D57" s="134"/>
-      <c r="E57" s="134"/>
-      <c r="F57" s="134"/>
-      <c r="G57" s="134" t="s">
-        <v>86</v>
-      </c>
-      <c r="H57" s="137"/>
-      <c r="I57" s="233" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A58" s="251"/>
-      <c r="B58" s="199" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="136"/>
-      <c r="D58" s="134"/>
-      <c r="E58" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="F58" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G58" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="H58" s="135" t="s">
-        <v>140</v>
-      </c>
-      <c r="I58" s="233" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="252"/>
-      <c r="B59" s="200" t="s">
+    <row r="60" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="174"/>
+      <c r="B60" s="148" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="133"/>
-      <c r="D59" s="131"/>
-      <c r="E59" s="131" t="s">
+      <c r="C60" s="149"/>
+      <c r="D60" s="150"/>
+      <c r="E60" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="F59" s="131" t="s">
+      <c r="F60" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="131" t="s">
+      <c r="G60" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="H59" s="132"/>
-      <c r="I59" s="235" t="s">
+      <c r="H60" s="150"/>
+      <c r="I60" s="151" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A60" s="253" t="s">
+    <row r="61" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="171" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="254" t="s">
+      <c r="B61" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="C60" s="255"/>
-      <c r="D60" s="256" t="s">
+      <c r="C61" s="127"/>
+      <c r="D61" s="126" t="s">
         <v>75</v>
       </c>
-      <c r="E60" s="256"/>
-      <c r="F60" s="256"/>
-      <c r="G60" s="256"/>
-      <c r="H60" s="257"/>
-      <c r="I60" s="258"/>
+      <c r="E61" s="126"/>
+      <c r="F61" s="126"/>
+      <c r="G61" s="126"/>
+      <c r="H61" s="126"/>
+      <c r="I61" s="134"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H60" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="10">
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A55"/>
-    <mergeCell ref="A56:A59"/>
+  <autoFilter ref="A1:H61" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="9">
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A57:A60"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A20:A42"/>
+    <mergeCell ref="A20:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="22" orientation="landscape" r:id="rId1"/>
@@ -3654,7 +3477,7 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
@@ -3686,7 +3509,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="111" t="s">
         <v>124</v>
       </c>
       <c r="B2" s="9"/>
@@ -3695,19 +3518,19 @@
       <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="188"/>
+      <c r="A3" s="112"/>
       <c r="B3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="188"/>
+      <c r="A4" s="112"/>
       <c r="B4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="188"/>
+      <c r="A5" s="112"/>
       <c r="B5" t="s">
         <v>39</v>
       </c>
@@ -3716,7 +3539,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="188"/>
+      <c r="A6" s="112"/>
       <c r="B6" t="s">
         <v>40</v>
       </c>
@@ -3725,7 +3548,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="188"/>
+      <c r="A7" s="112"/>
       <c r="B7" t="s">
         <v>41</v>
       </c>
@@ -3734,7 +3557,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="188"/>
+      <c r="A8" s="112"/>
       <c r="B8" t="s">
         <v>43</v>
       </c>
@@ -3743,7 +3566,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="189"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="11" t="s">
         <v>37</v>
       </c>
@@ -3754,7 +3577,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="187" t="s">
+      <c r="A10" s="111" t="s">
         <v>148</v>
       </c>
       <c r="B10" s="9"/>
@@ -3763,7 +3586,7 @@
       <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="188"/>
+      <c r="A11" s="112"/>
       <c r="B11" t="s">
         <v>46</v>
       </c>
@@ -3772,7 +3595,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="188"/>
+      <c r="A12" s="112"/>
       <c r="B12" t="s">
         <v>47</v>
       </c>
@@ -3781,13 +3604,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="188"/>
+      <c r="A13" s="112"/>
       <c r="B13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="189"/>
+      <c r="A14" s="113"/>
       <c r="B14" s="11" t="s">
         <v>96</v>
       </c>
@@ -3798,7 +3621,7 @@
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="187" t="s">
+      <c r="A15" s="111" t="s">
         <v>125</v>
       </c>
       <c r="B15" s="9"/>
@@ -3807,13 +3630,13 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="188"/>
+      <c r="A16" s="112"/>
       <c r="B16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="189"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="11" t="s">
         <v>50</v>
       </c>
@@ -3822,7 +3645,7 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="187" t="s">
+      <c r="A18" s="111" t="s">
         <v>149</v>
       </c>
       <c r="B18" s="9"/>
@@ -3831,7 +3654,7 @@
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="188"/>
+      <c r="A19" s="112"/>
       <c r="B19" t="s">
         <v>104</v>
       </c>
@@ -3840,7 +3663,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="188"/>
+      <c r="A20" s="112"/>
       <c r="B20" t="s">
         <v>103</v>
       </c>
@@ -3855,7 +3678,7 @@
       <c r="A24" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D27" s="190"/>
+      <c r="D27" s="114"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3979,7 +3802,7 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="186" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -3997,7 +3820,7 @@
       <c r="H5" s="71"/>
     </row>
     <row r="6" spans="1:11" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="117"/>
+      <c r="A6" s="187"/>
       <c r="B6" s="22"/>
       <c r="C6" s="23"/>
       <c r="D6" s="67"/>
@@ -4007,7 +3830,7 @@
       <c r="H6" s="72"/>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="188" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -4027,7 +3850,7 @@
       <c r="H7" s="71"/>
     </row>
     <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="119"/>
+      <c r="A8" s="189"/>
       <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
@@ -4045,7 +3868,7 @@
       <c r="H8" s="74"/>
     </row>
     <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="120"/>
+      <c r="A9" s="190"/>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
@@ -4077,7 +3900,7 @@
       <c r="H10" s="77"/>
     </row>
     <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="191" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="28" t="s">
@@ -4093,7 +3916,7 @@
       <c r="H11" s="79"/>
     </row>
     <row r="12" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="29" t="s">
         <v>6</v>
       </c>
@@ -4121,7 +3944,7 @@
       <c r="H13" s="77"/>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="186" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -4137,7 +3960,7 @@
       <c r="H14" s="79"/>
     </row>
     <row r="15" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="187"/>
       <c r="B15" s="19" t="s">
         <v>6</v>
       </c>
@@ -4153,7 +3976,7 @@
       <c r="H15" s="81"/>
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="123" t="s">
+      <c r="A16" s="193" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -4175,7 +3998,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="124"/>
+      <c r="A17" s="194"/>
       <c r="B17" s="36" t="s">
         <v>51</v>
       </c>
@@ -4197,7 +4020,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
+      <c r="A18" s="195"/>
       <c r="B18" s="37" t="s">
         <v>69</v>
       </c>
@@ -4231,7 +4054,7 @@
       <c r="H19" s="90"/>
     </row>
     <row r="20" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="179" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="43" t="s">
@@ -4249,7 +4072,7 @@
       <c r="H20" s="93"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="128"/>
+      <c r="A21" s="198"/>
       <c r="B21" s="39" t="s">
         <v>26</v>
       </c>
@@ -4271,7 +4094,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="128"/>
+      <c r="A22" s="198"/>
       <c r="B22" s="36" t="s">
         <v>27</v>
       </c>
@@ -4287,7 +4110,7 @@
       <c r="H22" s="85"/>
     </row>
     <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="128"/>
+      <c r="A23" s="198"/>
       <c r="B23" s="40" t="s">
         <v>89</v>
       </c>
@@ -4307,7 +4130,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="128"/>
+      <c r="A24" s="198"/>
       <c r="B24" s="36" t="s">
         <v>28</v>
       </c>
@@ -4325,7 +4148,7 @@
       <c r="H24" s="85"/>
     </row>
     <row r="25" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="128"/>
+      <c r="A25" s="198"/>
       <c r="B25" s="40" t="s">
         <v>29</v>
       </c>
@@ -4343,7 +4166,7 @@
       <c r="H25" s="85"/>
     </row>
     <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="128"/>
+      <c r="A26" s="198"/>
       <c r="B26" s="36" t="s">
         <v>30</v>
       </c>
@@ -4361,7 +4184,7 @@
       <c r="H26" s="85"/>
     </row>
     <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="128"/>
+      <c r="A27" s="198"/>
       <c r="B27" s="40" t="s">
         <v>31</v>
       </c>
@@ -4379,7 +4202,7 @@
       <c r="H27" s="85"/>
     </row>
     <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="128"/>
+      <c r="A28" s="198"/>
       <c r="B28" s="36" t="s">
         <v>58</v>
       </c>
@@ -4395,7 +4218,7 @@
       <c r="H28" s="85"/>
     </row>
     <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="128"/>
+      <c r="A29" s="198"/>
       <c r="B29" s="40" t="s">
         <v>32</v>
       </c>
@@ -4411,7 +4234,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="128"/>
+      <c r="A30" s="198"/>
       <c r="B30" s="36" t="s">
         <v>91</v>
       </c>
@@ -4427,7 +4250,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="128"/>
+      <c r="A31" s="198"/>
       <c r="B31" s="40" t="s">
         <v>92</v>
       </c>
@@ -4441,7 +4264,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="128"/>
+      <c r="A32" s="198"/>
       <c r="B32" s="36" t="s">
         <v>80</v>
       </c>
@@ -4457,7 +4280,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="128"/>
+      <c r="A33" s="198"/>
       <c r="B33" s="40" t="s">
         <v>33</v>
       </c>
@@ -4473,7 +4296,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="128"/>
+      <c r="A34" s="198"/>
       <c r="B34" s="36" t="s">
         <v>34</v>
       </c>
@@ -4487,7 +4310,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="128"/>
+      <c r="A35" s="198"/>
       <c r="B35" s="40" t="s">
         <v>67</v>
       </c>
@@ -4501,7 +4324,7 @@
       <c r="H35" s="85"/>
     </row>
     <row r="36" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="128"/>
+      <c r="A36" s="198"/>
       <c r="B36" s="41" t="s">
         <v>68</v>
       </c>
@@ -4515,7 +4338,7 @@
       <c r="H36" s="87"/>
     </row>
     <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="128"/>
+      <c r="A37" s="198"/>
       <c r="B37" s="40" t="s">
         <v>159</v>
       </c>
@@ -4533,7 +4356,7 @@
       <c r="H37" s="85"/>
     </row>
     <row r="38" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="110"/>
+      <c r="A38" s="180"/>
       <c r="B38" s="41" t="s">
         <v>161</v>
       </c>
@@ -4569,7 +4392,7 @@
       <c r="H39" s="90"/>
     </row>
     <row r="40" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="126" t="s">
+      <c r="A40" s="196" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="43" t="s">
@@ -4591,7 +4414,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="127"/>
+      <c r="A41" s="197"/>
       <c r="B41" s="37" t="s">
         <v>152</v>
       </c>
@@ -4611,7 +4434,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="109" t="s">
+      <c r="A42" s="179" t="s">
         <v>99</v>
       </c>
       <c r="B42" s="43" t="s">
@@ -4631,7 +4454,7 @@
       <c r="H42" s="97"/>
     </row>
     <row r="43" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="110"/>
+      <c r="A43" s="180"/>
       <c r="B43" s="37" t="s">
         <v>65</v>
       </c>
@@ -4647,7 +4470,7 @@
       <c r="H43" s="99"/>
     </row>
     <row r="44" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="181" t="s">
         <v>56</v>
       </c>
       <c r="B44" s="43" t="s">
@@ -4667,7 +4490,7 @@
       <c r="H44" s="97"/>
     </row>
     <row r="45" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="112"/>
+      <c r="A45" s="182"/>
       <c r="B45" s="40" t="s">
         <v>15</v>
       </c>
@@ -4687,7 +4510,7 @@
       <c r="H45" s="85"/>
     </row>
     <row r="46" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="112"/>
+      <c r="A46" s="182"/>
       <c r="B46" s="36" t="s">
         <v>16</v>
       </c>
@@ -4709,7 +4532,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="112"/>
+      <c r="A47" s="182"/>
       <c r="B47" s="40" t="s">
         <v>84</v>
       </c>
@@ -4725,7 +4548,7 @@
       <c r="H47" s="85"/>
     </row>
     <row r="48" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="112"/>
+      <c r="A48" s="182"/>
       <c r="B48" s="36" t="s">
         <v>18</v>
       </c>
@@ -4741,7 +4564,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="113"/>
+      <c r="A49" s="183"/>
       <c r="B49" s="37" t="s">
         <v>71</v>
       </c>
@@ -4755,7 +4578,7 @@
       <c r="H49" s="99"/>
     </row>
     <row r="50" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="114" t="s">
+      <c r="A50" s="184" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="43" t="s">
@@ -4779,7 +4602,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="114"/>
+      <c r="A51" s="184"/>
       <c r="B51" s="40" t="s">
         <v>152</v>
       </c>
@@ -4793,7 +4616,7 @@
       <c r="H51" s="85"/>
     </row>
     <row r="52" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="114"/>
+      <c r="A52" s="184"/>
       <c r="B52" s="36" t="s">
         <v>65</v>
       </c>
@@ -4813,7 +4636,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="115"/>
+      <c r="A53" s="185"/>
       <c r="B53" s="37" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Update to formatting of profile comparison
</commit_message>
<xml_diff>
--- a/input/images/CARINforBlueButtonProfileComparison.xlsx
+++ b/input/images/CARINforBlueButtonProfileComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cspears/dev/fhir/fsh/davinci/carin/carin-bb/input/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804C1B67-62C7-5E49-B9A8-931CC2B8B8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEE84AA-BE04-1D45-8AE0-DF0600438308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,9 +19,9 @@
     <sheet name="Other Profile Comparison - STU1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$H$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">EOBProfileComparison!$A$1:$I$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EOBProfileComparison - STU1'!$A$1:$H$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$I$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">EOBProfileComparison!$A$1:$I$73</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'EOBProfileComparison - STU1'!$A$1:$H$54</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Table32[#All]</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Table3[#All]</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="210">
   <si>
     <t>Pharmacy</t>
   </si>
@@ -662,24 +662,33 @@
     <t>billablePeriod</t>
   </si>
   <si>
-    <t>Period (provider statement period)</t>
-  </si>
-  <si>
-    <t>serviced[x]</t>
-  </si>
-  <si>
-    <t>date or period</t>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>servicedDate</t>
+  </si>
+  <si>
+    <t>servicePeriod</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>period</t>
   </si>
   <si>
     <t>date 
-(for individual procedure only, not for stay or complete encounter)</t>
+(for individual procedure only, not admission)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -757,8 +766,25 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,12 +878,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="8" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,7 +888,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1269,16 +1289,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1287,13 +1307,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1305,10 +1325,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1317,7 +1337,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -1335,10 +1355,21 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1347,7 +1378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1598,51 +1629,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="13" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="18" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1703,239 +1689,193 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="17" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="17" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="17" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="17" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="15" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="15" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2386,11 +2326,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72:I72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2401,7 +2341,7 @@
     <col min="4" max="9" width="29" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="51" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2430,1334 +2370,1429 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="161" t="s">
+      <c r="B2" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="150" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="163" t="s">
+      <c r="D2" s="138" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="165"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="54" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="95" t="s">
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="142"/>
+      <c r="K2" s="167"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="167" t="s">
+      <c r="B3" s="148"/>
+      <c r="C3" s="148" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="168" t="s">
+      <c r="D3" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="169" t="s">
+      <c r="E3" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="169" t="s">
+      <c r="F3" s="158" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="169" t="s">
+      <c r="G3" s="158" t="s">
         <v>181</v>
       </c>
-      <c r="H3" s="169" t="s">
+      <c r="H3" s="158" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="170" t="s">
+      <c r="I3" s="159" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="37" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="175" t="s">
+      <c r="K3" s="167"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="26" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="117" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="171"/>
-      <c r="C4" s="172" t="s">
+      <c r="B4" s="127"/>
+      <c r="C4" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="173"/>
-      <c r="E4" s="162" t="s">
+      <c r="D4" s="127"/>
+      <c r="E4" s="128" t="s">
         <v>179</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="128" t="s">
         <v>180</v>
       </c>
-      <c r="G4" s="162"/>
-      <c r="H4" s="173"/>
-      <c r="I4" s="174"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105" t="s">
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="129"/>
+      <c r="K4" s="167"/>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="176" t="s">
+      <c r="B5" s="149" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="177" t="s">
+      <c r="C5" s="152" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="178" t="s">
+      <c r="D5" s="160" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="178"/>
-      <c r="F5" s="178"/>
-      <c r="G5" s="178"/>
-      <c r="H5" s="178"/>
-      <c r="I5" s="179"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="105"/>
-      <c r="B6" s="180"/>
-      <c r="C6" s="181"/>
-      <c r="D6" s="182"/>
-      <c r="E6" s="182"/>
-      <c r="F6" s="182"/>
-      <c r="G6" s="182"/>
-      <c r="H6" s="182"/>
-      <c r="I6" s="65"/>
-    </row>
-    <row r="7" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="161"/>
+      <c r="K5" s="167"/>
+    </row>
+    <row r="6" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="178" t="s">
+      <c r="B6" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="177"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178" t="s">
+      <c r="C6" s="151"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127" t="s">
         <v>113</v>
       </c>
-      <c r="F7" s="178" t="s">
+      <c r="F6" s="127" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="178" t="s">
+      <c r="G6" s="127" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="178"/>
-      <c r="I7" s="179" t="s">
+      <c r="H6" s="127"/>
+      <c r="I6" s="135" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106"/>
-      <c r="B8" s="131" t="s">
+      <c r="K6" s="167"/>
+    </row>
+    <row r="7" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="119"/>
+      <c r="B7" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="129"/>
-      <c r="D8" s="130"/>
-      <c r="E8" s="130" t="s">
+      <c r="C7" s="153"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="130" t="s">
+      <c r="F7" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="130" t="s">
+      <c r="G7" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="132"/>
-      <c r="I8" s="143" t="s">
+      <c r="H7" s="168"/>
+      <c r="I7" s="164" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
-      <c r="B9" s="183" t="s">
+      <c r="K7" s="167"/>
+    </row>
+    <row r="8" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="119"/>
+      <c r="B8" s="136" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="184" t="s">
+      <c r="C8" s="154" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="183"/>
-      <c r="E9" s="183" t="s">
+      <c r="D8" s="136"/>
+      <c r="E8" s="136" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="183"/>
-      <c r="G9" s="183"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="185"/>
-    </row>
-    <row r="10" spans="1:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="96" t="s">
+      <c r="F8" s="136"/>
+      <c r="G8" s="136"/>
+      <c r="H8" s="136"/>
+      <c r="I8" s="137"/>
+      <c r="K8" s="167"/>
+    </row>
+    <row r="9" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="186" t="s">
+      <c r="B9" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="172"/>
-      <c r="D10" s="173" t="s">
+      <c r="C9" s="152"/>
+      <c r="D9" s="160" t="s">
         <v>126</v>
       </c>
-      <c r="E10" s="187"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="187"/>
-      <c r="I10" s="69"/>
-    </row>
-    <row r="11" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="107" t="s">
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="169"/>
+      <c r="H9" s="169"/>
+      <c r="I9" s="170"/>
+      <c r="K9" s="167"/>
+    </row>
+    <row r="10" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="178" t="s">
+      <c r="B10" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="177"/>
-      <c r="D11" s="188"/>
-      <c r="E11" s="188" t="s">
+      <c r="C10" s="151"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="188"/>
-      <c r="G11" s="188"/>
-      <c r="H11" s="188"/>
-      <c r="I11" s="189"/>
-    </row>
-    <row r="12" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
-      <c r="B12" s="131" t="s">
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="129"/>
+      <c r="K10" s="167"/>
+    </row>
+    <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="120"/>
+      <c r="B11" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="129"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133" t="s">
+      <c r="C11" s="153"/>
+      <c r="D11" s="171"/>
+      <c r="E11" s="171" t="s">
         <v>150</v>
       </c>
-      <c r="F12" s="135"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="135"/>
-      <c r="I12" s="144"/>
-    </row>
-    <row r="13" spans="1:9" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
-      <c r="B13" s="183" t="s">
+      <c r="F11" s="171"/>
+      <c r="G11" s="171"/>
+      <c r="H11" s="171"/>
+      <c r="I11" s="172"/>
+      <c r="K11" s="167"/>
+    </row>
+    <row r="12" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="120"/>
+      <c r="B12" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="184"/>
-      <c r="D13" s="190"/>
-      <c r="E13" s="192" t="s">
+      <c r="C12" s="154"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="145" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="144"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="146"/>
+      <c r="K12" s="167"/>
+    </row>
+    <row r="13" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="130"/>
+      <c r="C13" s="152"/>
+      <c r="D13" s="160" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="169"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="170"/>
+      <c r="K13" s="167"/>
+    </row>
+    <row r="14" spans="1:11" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="118" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="127" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="151"/>
+      <c r="D14" s="147" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128"/>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="129"/>
+      <c r="K14" s="167"/>
+    </row>
+    <row r="15" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="118"/>
+      <c r="B15" s="134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="155" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="165" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="174"/>
+      <c r="K15" s="167"/>
+    </row>
+    <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="121" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="127" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="151"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="128" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" s="128"/>
+      <c r="G16" s="128"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="129"/>
+      <c r="K16" s="167"/>
+    </row>
+    <row r="17" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="115"/>
+      <c r="B17" s="134" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="155"/>
+      <c r="D17" s="165"/>
+      <c r="E17" s="165" t="s">
+        <v>207</v>
+      </c>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="166"/>
+      <c r="K17" s="167"/>
+    </row>
+    <row r="18" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="122" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="127" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="151"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="127" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="127" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="127" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="135" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="167"/>
+    </row>
+    <row r="19" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="122"/>
+      <c r="B19" s="131" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="153"/>
+      <c r="D19" s="163" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="163" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="163" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="163" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="163" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="164" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="167"/>
+    </row>
+    <row r="20" spans="1:11" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="122"/>
+      <c r="B20" s="136" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="154" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136" t="s">
+        <v>182</v>
+      </c>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="137"/>
+      <c r="K20" s="167"/>
+    </row>
+    <row r="21" spans="1:11" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="130"/>
+      <c r="C21" s="152"/>
+      <c r="D21" s="160" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="160" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="160" t="s">
+        <v>151</v>
+      </c>
+      <c r="G21" s="160"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="162" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" s="167"/>
+    </row>
+    <row r="22" spans="1:11" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="127" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="151" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="127" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="135"/>
+      <c r="K22" s="167"/>
+    </row>
+    <row r="23" spans="1:11" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="123"/>
+      <c r="B23" s="131" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="153"/>
+      <c r="D23" s="163"/>
+      <c r="E23" s="163" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="163"/>
+      <c r="G23" s="163"/>
+      <c r="H23" s="163"/>
+      <c r="I23" s="164"/>
+      <c r="K23" s="167"/>
+    </row>
+    <row r="24" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="123"/>
+      <c r="B24" s="132" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="156"/>
+      <c r="D24" s="132"/>
+      <c r="E24" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="133" t="s">
+        <v>2</v>
+      </c>
+      <c r="K24" s="167"/>
+    </row>
+    <row r="25" spans="1:11" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="123"/>
+      <c r="B25" s="131" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="153" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="163"/>
+      <c r="E25" s="163" t="s">
+        <v>131</v>
+      </c>
+      <c r="F25" s="163" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="163"/>
+      <c r="H25" s="163"/>
+      <c r="I25" s="164"/>
+      <c r="K25" s="167"/>
+    </row>
+    <row r="26" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="123"/>
+      <c r="B26" s="132" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="156" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="132"/>
+      <c r="E26" s="132" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="132" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="132"/>
+      <c r="H26" s="132"/>
+      <c r="I26" s="133"/>
+      <c r="K26" s="167"/>
+    </row>
+    <row r="27" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="123"/>
+      <c r="B27" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="153" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="163"/>
+      <c r="E27" s="163" t="s">
+        <v>133</v>
+      </c>
+      <c r="F27" s="163" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" s="163"/>
+      <c r="H27" s="163"/>
+      <c r="I27" s="164"/>
+      <c r="K27" s="167"/>
+    </row>
+    <row r="28" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="123"/>
+      <c r="B28" s="132" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="156" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="132"/>
+      <c r="E28" s="132" t="s">
+        <v>134</v>
+      </c>
+      <c r="F28" s="132" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" s="132"/>
+      <c r="H28" s="132"/>
+      <c r="I28" s="133"/>
+      <c r="K28" s="167"/>
+    </row>
+    <row r="29" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="123"/>
+      <c r="B29" s="131" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="153" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="163"/>
+      <c r="E29" s="163" t="s">
+        <v>135</v>
+      </c>
+      <c r="F29" s="163"/>
+      <c r="G29" s="163"/>
+      <c r="H29" s="163"/>
+      <c r="I29" s="164"/>
+      <c r="K29" s="167"/>
+    </row>
+    <row r="30" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="123"/>
+      <c r="B30" s="132" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="156"/>
+      <c r="D30" s="132"/>
+      <c r="E30" s="132"/>
+      <c r="F30" s="132"/>
+      <c r="G30" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="132"/>
+      <c r="I30" s="133"/>
+      <c r="K30" s="167"/>
+    </row>
+    <row r="31" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="123"/>
+      <c r="B31" s="131" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="153" t="s">
+        <v>199</v>
+      </c>
+      <c r="D31" s="163"/>
+      <c r="E31" s="163"/>
+      <c r="F31" s="163"/>
+      <c r="G31" s="163" t="s">
+        <v>200</v>
+      </c>
+      <c r="H31" s="163"/>
+      <c r="I31" s="164"/>
+      <c r="K31" s="167"/>
+    </row>
+    <row r="32" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="123"/>
+      <c r="B32" s="132" t="s">
+        <v>198</v>
+      </c>
+      <c r="C32" s="156"/>
+      <c r="D32" s="132"/>
+      <c r="E32" s="132"/>
+      <c r="F32" s="132"/>
+      <c r="G32" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="132"/>
+      <c r="I32" s="133"/>
+      <c r="K32" s="167"/>
+    </row>
+    <row r="33" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="123"/>
+      <c r="B33" s="131" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" s="153"/>
+      <c r="D33" s="163"/>
+      <c r="E33" s="163"/>
+      <c r="F33" s="163"/>
+      <c r="G33" s="163" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" s="163"/>
+      <c r="I33" s="164"/>
+      <c r="K33" s="167"/>
+    </row>
+    <row r="34" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="123"/>
+      <c r="B34" s="132" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" s="156"/>
+      <c r="D34" s="132"/>
+      <c r="E34" s="132"/>
+      <c r="F34" s="132"/>
+      <c r="G34" s="132" t="s">
+        <v>160</v>
+      </c>
+      <c r="H34" s="132"/>
+      <c r="I34" s="133"/>
+      <c r="K34" s="167"/>
+    </row>
+    <row r="35" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="123"/>
+      <c r="B35" s="131" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="153"/>
+      <c r="D35" s="163"/>
+      <c r="E35" s="163"/>
+      <c r="F35" s="163"/>
+      <c r="G35" s="163" t="s">
+        <v>160</v>
+      </c>
+      <c r="H35" s="163"/>
+      <c r="I35" s="164"/>
+      <c r="K35" s="167"/>
+    </row>
+    <row r="36" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="123"/>
+      <c r="B36" s="132" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="156"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="132"/>
+      <c r="G36" s="132" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="132"/>
+      <c r="I36" s="133"/>
+      <c r="K36" s="167"/>
+    </row>
+    <row r="37" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="123"/>
+      <c r="B37" s="131" t="s">
+        <v>187</v>
+      </c>
+      <c r="C37" s="153" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="163"/>
+      <c r="E37" s="163"/>
+      <c r="F37" s="163"/>
+      <c r="G37" s="163"/>
+      <c r="H37" s="163" t="s">
+        <v>136</v>
+      </c>
+      <c r="I37" s="164"/>
+      <c r="K37" s="167"/>
+    </row>
+    <row r="38" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="123"/>
+      <c r="B38" s="132" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="132"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="132"/>
+      <c r="G38" s="132"/>
+      <c r="H38" s="132" t="s">
+        <v>137</v>
+      </c>
+      <c r="I38" s="133"/>
+      <c r="K38" s="167"/>
+    </row>
+    <row r="39" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="123"/>
+      <c r="B39" s="131" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="153"/>
+      <c r="D39" s="163"/>
+      <c r="E39" s="163"/>
+      <c r="F39" s="163"/>
+      <c r="G39" s="163"/>
+      <c r="H39" s="163" t="s">
+        <v>3</v>
+      </c>
+      <c r="I39" s="164"/>
+      <c r="K39" s="167"/>
+    </row>
+    <row r="40" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="123"/>
+      <c r="B40" s="132" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="156"/>
+      <c r="D40" s="132"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="132"/>
+      <c r="G40" s="132"/>
+      <c r="H40" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="I40" s="133"/>
+      <c r="K40" s="167"/>
+    </row>
+    <row r="41" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="123"/>
+      <c r="B41" s="131" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="153" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="163"/>
+      <c r="E41" s="163"/>
+      <c r="F41" s="163"/>
+      <c r="G41" s="163"/>
+      <c r="H41" s="163" t="s">
+        <v>138</v>
+      </c>
+      <c r="I41" s="164"/>
+      <c r="K41" s="167"/>
+    </row>
+    <row r="42" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="123"/>
+      <c r="B42" s="132" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="132"/>
+      <c r="E42" s="132"/>
+      <c r="F42" s="132"/>
+      <c r="G42" s="132"/>
+      <c r="H42" s="132" t="s">
+        <v>139</v>
+      </c>
+      <c r="I42" s="133"/>
+      <c r="K42" s="167"/>
+    </row>
+    <row r="43" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="123"/>
+      <c r="B43" s="131" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="153"/>
+      <c r="D43" s="163"/>
+      <c r="E43" s="163"/>
+      <c r="F43" s="163"/>
+      <c r="G43" s="163"/>
+      <c r="H43" s="163" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" s="164"/>
+      <c r="K43" s="167"/>
+    </row>
+    <row r="44" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="123"/>
+      <c r="B44" s="132" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="156"/>
+      <c r="D44" s="132"/>
+      <c r="E44" s="132"/>
+      <c r="F44" s="132"/>
+      <c r="G44" s="132" t="s">
+        <v>142</v>
+      </c>
+      <c r="H44" s="132"/>
+      <c r="I44" s="133" t="s">
+        <v>142</v>
+      </c>
+      <c r="K44" s="167"/>
+    </row>
+    <row r="45" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="123"/>
+      <c r="B45" s="131" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="153"/>
+      <c r="D45" s="163"/>
+      <c r="E45" s="163" t="s">
+        <v>160</v>
+      </c>
+      <c r="F45" s="163" t="s">
+        <v>160</v>
+      </c>
+      <c r="G45" s="163" t="s">
+        <v>160</v>
+      </c>
+      <c r="H45" s="163"/>
+      <c r="I45" s="164" t="s">
+        <v>160</v>
+      </c>
+      <c r="K45" s="167"/>
+    </row>
+    <row r="46" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="123"/>
+      <c r="B46" s="132" t="s">
+        <v>174</v>
+      </c>
+      <c r="C46" s="156"/>
+      <c r="D46" s="132"/>
+      <c r="E46" s="132" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" s="132" t="s">
+        <v>160</v>
+      </c>
+      <c r="G46" s="132" t="s">
+        <v>160</v>
+      </c>
+      <c r="H46" s="132"/>
+      <c r="I46" s="133" t="s">
+        <v>160</v>
+      </c>
+      <c r="K46" s="167"/>
+    </row>
+    <row r="47" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="123"/>
+      <c r="B47" s="131" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" s="153"/>
+      <c r="D47" s="163"/>
+      <c r="E47" s="163"/>
+      <c r="F47" s="163"/>
+      <c r="G47" s="163"/>
+      <c r="H47" s="163"/>
+      <c r="I47" s="164" t="s">
+        <v>172</v>
+      </c>
+      <c r="K47" s="167"/>
+    </row>
+    <row r="48" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="123"/>
+      <c r="B48" s="132" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="156"/>
+      <c r="D48" s="132"/>
+      <c r="E48" s="132"/>
+      <c r="F48" s="132"/>
+      <c r="G48" s="132"/>
+      <c r="H48" s="132"/>
+      <c r="I48" s="133" t="s">
+        <v>170</v>
+      </c>
+      <c r="K48" s="167"/>
+    </row>
+    <row r="49" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="123"/>
+      <c r="B49" s="131" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="153" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="163"/>
+      <c r="E49" s="163"/>
+      <c r="F49" s="163"/>
+      <c r="G49" s="163"/>
+      <c r="H49" s="163"/>
+      <c r="I49" s="164" t="s">
+        <v>165</v>
+      </c>
+      <c r="K49" s="167"/>
+    </row>
+    <row r="50" spans="1:11" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="123"/>
+      <c r="B50" s="136" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="154" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="136"/>
+      <c r="E50" s="136"/>
+      <c r="F50" s="136"/>
+      <c r="G50" s="136"/>
+      <c r="H50" s="136"/>
+      <c r="I50" s="137" t="s">
+        <v>167</v>
+      </c>
+      <c r="K50" s="167"/>
+    </row>
+    <row r="51" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="130" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="152" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" s="160" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51" s="160"/>
+      <c r="F51" s="160"/>
+      <c r="G51" s="160"/>
+      <c r="H51" s="160"/>
+      <c r="I51" s="162"/>
+      <c r="K51" s="167"/>
+    </row>
+    <row r="52" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="114" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="138" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="150"/>
+      <c r="D52" s="138"/>
+      <c r="E52" s="138" t="s">
+        <v>140</v>
+      </c>
+      <c r="F52" s="138" t="s">
+        <v>140</v>
+      </c>
+      <c r="G52" s="138" t="s">
+        <v>140</v>
+      </c>
+      <c r="H52" s="138" t="s">
+        <v>140</v>
+      </c>
+      <c r="I52" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="K52" s="167"/>
+    </row>
+    <row r="53" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="123" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" s="140" t="s">
+        <v>190</v>
+      </c>
+      <c r="C53" s="157" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="175"/>
+      <c r="E53" s="175" t="s">
+        <v>119</v>
+      </c>
+      <c r="F53" s="175" t="s">
+        <v>119</v>
+      </c>
+      <c r="G53" s="175" t="s">
+        <v>119</v>
+      </c>
+      <c r="H53" s="175" t="s">
+        <v>119</v>
+      </c>
+      <c r="I53" s="176" t="s">
+        <v>119</v>
+      </c>
+      <c r="K53" s="167"/>
+    </row>
+    <row r="54" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="123"/>
+      <c r="B54" s="132" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="156" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" s="132"/>
+      <c r="E54" s="132"/>
+      <c r="F54" s="132"/>
+      <c r="G54" s="132" t="s">
+        <v>119</v>
+      </c>
+      <c r="H54" s="132"/>
+      <c r="I54" s="133" t="s">
+        <v>119</v>
+      </c>
+      <c r="K54" s="167"/>
+    </row>
+    <row r="55" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="123"/>
+      <c r="B55" s="131" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="153" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="163"/>
+      <c r="E55" s="163" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" s="163" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="163" t="s">
+        <v>141</v>
+      </c>
+      <c r="H55" s="163" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" s="164" t="s">
+        <v>141</v>
+      </c>
+      <c r="K55" s="167"/>
+    </row>
+    <row r="56" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="123"/>
+      <c r="B56" s="132" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="156"/>
+      <c r="D56" s="132"/>
+      <c r="E56" s="132" t="s">
+        <v>140</v>
+      </c>
+      <c r="F56" s="132" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" s="132"/>
+      <c r="H56" s="132"/>
+      <c r="I56" s="133"/>
+      <c r="K56" s="167"/>
+    </row>
+    <row r="57" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="123"/>
+      <c r="B57" s="134" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" s="155" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="165"/>
+      <c r="E57" s="165" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="165" t="s">
+        <v>90</v>
+      </c>
+      <c r="G57" s="165"/>
+      <c r="H57" s="165"/>
+      <c r="I57" s="166"/>
+      <c r="K57" s="167"/>
+    </row>
+    <row r="58" spans="1:11" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="124" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="127" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="151" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="127"/>
+      <c r="E58" s="127" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="127" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" s="127"/>
+      <c r="H58" s="127"/>
+      <c r="I58" s="135"/>
+      <c r="K58" s="167"/>
+    </row>
+    <row r="59" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="124"/>
+      <c r="B59" s="131" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="153" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="163"/>
+      <c r="E59" s="163" t="s">
+        <v>144</v>
+      </c>
+      <c r="F59" s="163" t="s">
+        <v>144</v>
+      </c>
+      <c r="G59" s="163" t="s">
+        <v>144</v>
+      </c>
+      <c r="H59" s="163"/>
+      <c r="I59" s="164" t="s">
+        <v>144</v>
+      </c>
+      <c r="K59" s="167"/>
+    </row>
+    <row r="60" spans="1:11" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="124"/>
+      <c r="B60" s="132" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" s="132"/>
+      <c r="E60" s="132" t="s">
+        <v>154</v>
+      </c>
+      <c r="F60" s="132" t="s">
+        <v>154</v>
+      </c>
+      <c r="G60" s="132" t="s">
+        <v>185</v>
+      </c>
+      <c r="H60" s="132" t="s">
+        <v>109</v>
+      </c>
+      <c r="I60" s="133" t="s">
+        <v>145</v>
+      </c>
+      <c r="K60" s="167"/>
+    </row>
+    <row r="61" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="124"/>
+      <c r="B61" s="131" t="s">
+        <v>205</v>
+      </c>
+      <c r="C61" s="153"/>
+      <c r="D61" s="163"/>
+      <c r="E61" s="163"/>
+      <c r="F61" s="163" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="163" t="s">
+        <v>2</v>
+      </c>
+      <c r="H61" s="163" t="s">
+        <v>2</v>
+      </c>
+      <c r="I61" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="K61" s="167"/>
+    </row>
+    <row r="62" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="124"/>
+      <c r="B62" s="132" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="190"/>
-      <c r="G13" s="190"/>
-      <c r="H13" s="190"/>
-      <c r="I13" s="191"/>
-    </row>
-    <row r="14" spans="1:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="186"/>
-      <c r="C14" s="172"/>
-      <c r="D14" s="173" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="187"/>
-      <c r="F14" s="187"/>
-      <c r="G14" s="187"/>
-      <c r="H14" s="187"/>
-      <c r="I14" s="69"/>
-    </row>
-    <row r="15" spans="1:9" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="105" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="178" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="193" t="s">
-        <v>188</v>
-      </c>
-      <c r="E15" s="188"/>
-      <c r="F15" s="188"/>
-      <c r="G15" s="188"/>
-      <c r="H15" s="188"/>
-      <c r="I15" s="189"/>
-    </row>
-    <row r="16" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="180" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="181" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="182" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="194"/>
-      <c r="F16" s="194"/>
-      <c r="G16" s="194"/>
-      <c r="H16" s="194"/>
-      <c r="I16" s="73"/>
-    </row>
-    <row r="17" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="101" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" s="168"/>
-      <c r="C17" s="169"/>
-      <c r="D17" s="168"/>
-      <c r="E17" s="195" t="s">
-        <v>203</v>
-      </c>
-      <c r="F17" s="195"/>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="196"/>
-    </row>
-    <row r="18" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="108" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="197" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="198"/>
-      <c r="D18" s="199"/>
-      <c r="E18" s="200" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" s="199" t="s">
-        <v>116</v>
-      </c>
-      <c r="G18" s="199" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" s="200" t="s">
-        <v>118</v>
-      </c>
-      <c r="I18" s="201" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="108"/>
-      <c r="B19" s="136" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="137"/>
-      <c r="D19" s="136" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" s="136" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="136" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="136" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="136" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="145" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="108"/>
-      <c r="B20" s="148" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="149" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150" t="s">
-        <v>182</v>
-      </c>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
-      <c r="I20" s="76"/>
-    </row>
-    <row r="21" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="98" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="202"/>
-      <c r="C21" s="203"/>
-      <c r="D21" s="202" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="202" t="s">
-        <v>151</v>
-      </c>
-      <c r="F21" s="202" t="s">
-        <v>151</v>
-      </c>
-      <c r="G21" s="204"/>
-      <c r="H21" s="204"/>
-      <c r="I21" s="205" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="102" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="206" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="207" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="208" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="209"/>
-      <c r="F22" s="209"/>
-      <c r="G22" s="210"/>
-      <c r="H22" s="210"/>
-      <c r="I22" s="211"/>
-    </row>
-    <row r="23" spans="1:9" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="102"/>
-      <c r="B23" s="134" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="137"/>
-      <c r="D23" s="142"/>
-      <c r="E23" s="134" t="s">
-        <v>183</v>
-      </c>
-      <c r="F23" s="136"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="141"/>
-      <c r="I23" s="147"/>
-    </row>
-    <row r="24" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="102"/>
-      <c r="B24" s="138" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="139"/>
-      <c r="D24" s="140"/>
-      <c r="E24" s="140" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="140" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" s="140" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="140" t="s">
-        <v>2</v>
-      </c>
-      <c r="I24" s="146" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="102"/>
-      <c r="B25" s="136" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="137" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="136"/>
-      <c r="E25" s="136" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="136" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" s="136"/>
-      <c r="H25" s="136"/>
-      <c r="I25" s="145"/>
-    </row>
-    <row r="26" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="102"/>
-      <c r="B26" s="138" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="139" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="140"/>
-      <c r="E26" s="140" t="s">
-        <v>132</v>
-      </c>
-      <c r="F26" s="140" t="s">
-        <v>132</v>
-      </c>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="146"/>
-    </row>
-    <row r="27" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="102"/>
-      <c r="B27" s="136" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="137" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="136" t="s">
-        <v>133</v>
-      </c>
-      <c r="G27" s="136"/>
-      <c r="H27" s="136"/>
-      <c r="I27" s="145"/>
-    </row>
-    <row r="28" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="102"/>
-      <c r="B28" s="138" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="139" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="140"/>
-      <c r="E28" s="140" t="s">
-        <v>134</v>
-      </c>
-      <c r="F28" s="140" t="s">
-        <v>134</v>
-      </c>
-      <c r="G28" s="140"/>
-      <c r="H28" s="140"/>
-      <c r="I28" s="146"/>
-    </row>
-    <row r="29" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="102"/>
-      <c r="B29" s="136" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="137" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="136"/>
-      <c r="G29" s="136"/>
-      <c r="H29" s="136"/>
-      <c r="I29" s="145"/>
-    </row>
-    <row r="30" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="102"/>
-      <c r="B30" s="138" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="139"/>
-      <c r="D30" s="140"/>
-      <c r="E30" s="140"/>
-      <c r="F30" s="140"/>
-      <c r="G30" s="140" t="s">
-        <v>3</v>
-      </c>
-      <c r="H30" s="140"/>
-      <c r="I30" s="146"/>
-    </row>
-    <row r="31" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="102"/>
-      <c r="B31" s="136" t="s">
-        <v>193</v>
-      </c>
-      <c r="C31" s="137" t="s">
-        <v>199</v>
-      </c>
-      <c r="D31" s="136"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="136"/>
-      <c r="G31" s="136" t="s">
-        <v>200</v>
-      </c>
-      <c r="H31" s="136"/>
-      <c r="I31" s="145"/>
-    </row>
-    <row r="32" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="102"/>
-      <c r="B32" s="138" t="s">
-        <v>198</v>
-      </c>
-      <c r="C32" s="139"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="140"/>
-      <c r="G32" s="140" t="s">
-        <v>3</v>
-      </c>
-      <c r="H32" s="140"/>
-      <c r="I32" s="146"/>
-    </row>
-    <row r="33" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="102"/>
-      <c r="B33" s="136" t="s">
-        <v>194</v>
-      </c>
-      <c r="C33" s="137"/>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="136" t="s">
-        <v>160</v>
-      </c>
-      <c r="H33" s="136"/>
-      <c r="I33" s="145"/>
-    </row>
-    <row r="34" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="102"/>
-      <c r="B34" s="138" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34" s="139"/>
-      <c r="D34" s="140"/>
-      <c r="E34" s="140"/>
-      <c r="F34" s="140"/>
-      <c r="G34" s="140" t="s">
-        <v>160</v>
-      </c>
-      <c r="H34" s="140"/>
-      <c r="I34" s="146"/>
-    </row>
-    <row r="35" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="102"/>
-      <c r="B35" s="136" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35" s="137"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
-      <c r="F35" s="136"/>
-      <c r="G35" s="136" t="s">
-        <v>160</v>
-      </c>
-      <c r="H35" s="136"/>
-      <c r="I35" s="145"/>
-    </row>
-    <row r="36" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="102"/>
-      <c r="B36" s="138" t="s">
-        <v>197</v>
-      </c>
-      <c r="C36" s="139"/>
-      <c r="D36" s="140"/>
-      <c r="E36" s="140"/>
-      <c r="F36" s="140"/>
-      <c r="G36" s="140" t="s">
-        <v>160</v>
-      </c>
-      <c r="H36" s="140"/>
-      <c r="I36" s="146"/>
-    </row>
-    <row r="37" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="102"/>
-      <c r="B37" s="136" t="s">
-        <v>187</v>
-      </c>
-      <c r="C37" s="137" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="136"/>
-      <c r="F37" s="136"/>
-      <c r="G37" s="136"/>
-      <c r="H37" s="136" t="s">
-        <v>136</v>
-      </c>
-      <c r="I37" s="145"/>
-    </row>
-    <row r="38" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="102"/>
-      <c r="B38" s="138" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" s="139" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="140"/>
-      <c r="E38" s="140"/>
-      <c r="F38" s="140"/>
-      <c r="G38" s="140"/>
-      <c r="H38" s="140" t="s">
-        <v>137</v>
-      </c>
-      <c r="I38" s="146"/>
-    </row>
-    <row r="39" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="102"/>
-      <c r="B39" s="136" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" s="137"/>
-      <c r="D39" s="136"/>
-      <c r="E39" s="136"/>
-      <c r="F39" s="136"/>
-      <c r="G39" s="136"/>
-      <c r="H39" s="136" t="s">
-        <v>3</v>
-      </c>
-      <c r="I39" s="145"/>
-    </row>
-    <row r="40" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="102"/>
-      <c r="B40" s="138" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="139"/>
-      <c r="D40" s="140"/>
-      <c r="E40" s="140"/>
-      <c r="F40" s="140"/>
-      <c r="G40" s="140"/>
-      <c r="H40" s="140" t="s">
-        <v>3</v>
-      </c>
-      <c r="I40" s="146"/>
-    </row>
-    <row r="41" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="102"/>
-      <c r="B41" s="136" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="137" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="136"/>
-      <c r="E41" s="136"/>
-      <c r="F41" s="136"/>
-      <c r="G41" s="136"/>
-      <c r="H41" s="136" t="s">
-        <v>138</v>
-      </c>
-      <c r="I41" s="145"/>
-    </row>
-    <row r="42" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="102"/>
-      <c r="B42" s="138" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="139" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="140"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="140"/>
-      <c r="G42" s="140"/>
-      <c r="H42" s="140" t="s">
-        <v>139</v>
-      </c>
-      <c r="I42" s="146"/>
-    </row>
-    <row r="43" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="102"/>
-      <c r="B43" s="136" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="137"/>
-      <c r="D43" s="136"/>
-      <c r="E43" s="136"/>
-      <c r="F43" s="136"/>
-      <c r="G43" s="136"/>
-      <c r="H43" s="136" t="s">
-        <v>3</v>
-      </c>
-      <c r="I43" s="145"/>
-    </row>
-    <row r="44" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="102"/>
-      <c r="B44" s="138" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" s="139"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140" t="s">
-        <v>142</v>
-      </c>
-      <c r="H44" s="140"/>
-      <c r="I44" s="146" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="102"/>
-      <c r="B45" s="136" t="s">
-        <v>161</v>
-      </c>
-      <c r="C45" s="137"/>
-      <c r="D45" s="136"/>
-      <c r="E45" s="136" t="s">
-        <v>160</v>
-      </c>
-      <c r="F45" s="136" t="s">
-        <v>160</v>
-      </c>
-      <c r="G45" s="136" t="s">
-        <v>160</v>
-      </c>
-      <c r="H45" s="136"/>
-      <c r="I45" s="145" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="102"/>
-      <c r="B46" s="138" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="139"/>
-      <c r="D46" s="140"/>
-      <c r="E46" s="140" t="s">
-        <v>160</v>
-      </c>
-      <c r="F46" s="140" t="s">
-        <v>160</v>
-      </c>
-      <c r="G46" s="140" t="s">
-        <v>160</v>
-      </c>
-      <c r="H46" s="140"/>
-      <c r="I46" s="146" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="102"/>
-      <c r="B47" s="136" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="137"/>
-      <c r="D47" s="136"/>
-      <c r="E47" s="136"/>
-      <c r="F47" s="136"/>
-      <c r="G47" s="136"/>
-      <c r="H47" s="136"/>
-      <c r="I47" s="145" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="102"/>
-      <c r="B48" s="138" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="139"/>
-      <c r="D48" s="140"/>
-      <c r="E48" s="140"/>
-      <c r="F48" s="140"/>
-      <c r="G48" s="140"/>
-      <c r="H48" s="140"/>
-      <c r="I48" s="146" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="102"/>
-      <c r="B49" s="136" t="s">
-        <v>169</v>
-      </c>
-      <c r="C49" s="137" t="s">
+      <c r="C62" s="156"/>
+      <c r="D62" s="132"/>
+      <c r="E62" s="132"/>
+      <c r="F62" s="132"/>
+      <c r="G62" s="132" t="s">
+        <v>208</v>
+      </c>
+      <c r="H62" s="132"/>
+      <c r="I62" s="133" t="s">
+        <v>208</v>
+      </c>
+      <c r="K62" s="167"/>
+    </row>
+    <row r="63" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="124"/>
+      <c r="B63" s="131" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="153" t="s">
         <v>163</v>
       </c>
-      <c r="D49" s="136"/>
-      <c r="E49" s="136"/>
-      <c r="F49" s="136"/>
-      <c r="G49" s="136"/>
-      <c r="H49" s="136"/>
-      <c r="I49" s="145" t="s">
+      <c r="D63" s="163"/>
+      <c r="E63" s="163"/>
+      <c r="F63" s="163"/>
+      <c r="G63" s="163" t="s">
+        <v>147</v>
+      </c>
+      <c r="H63" s="163"/>
+      <c r="I63" s="164" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="102"/>
-      <c r="B50" s="148" t="s">
-        <v>168</v>
-      </c>
-      <c r="C50" s="149" t="s">
+      <c r="K63" s="167"/>
+    </row>
+    <row r="64" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="124"/>
+      <c r="B64" s="132" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="156" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="150"/>
-      <c r="E50" s="150"/>
-      <c r="F50" s="150"/>
-      <c r="G50" s="150"/>
-      <c r="H50" s="150"/>
-      <c r="I50" s="76" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="99" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="202" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="203" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="202" t="s">
-        <v>88</v>
-      </c>
-      <c r="E51" s="202"/>
-      <c r="F51" s="202"/>
-      <c r="G51" s="202"/>
-      <c r="H51" s="202"/>
-      <c r="I51" s="205"/>
-    </row>
-    <row r="52" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="100" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="212" t="s">
+      <c r="D64" s="132"/>
+      <c r="E64" s="132"/>
+      <c r="F64" s="132"/>
+      <c r="G64" s="132"/>
+      <c r="H64" s="132"/>
+      <c r="I64" s="133" t="s">
+        <v>162</v>
+      </c>
+      <c r="K64" s="167"/>
+    </row>
+    <row r="65" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="124"/>
+      <c r="B65" s="131" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" s="153" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="163"/>
+      <c r="E65" s="163"/>
+      <c r="F65" s="163"/>
+      <c r="G65" s="163" t="s">
+        <v>147</v>
+      </c>
+      <c r="H65" s="163"/>
+      <c r="I65" s="164" t="s">
+        <v>147</v>
+      </c>
+      <c r="K65" s="167"/>
+    </row>
+    <row r="66" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="124"/>
+      <c r="B66" s="132" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="156" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="132"/>
+      <c r="E66" s="132"/>
+      <c r="F66" s="132"/>
+      <c r="G66" s="132"/>
+      <c r="H66" s="132" t="s">
+        <v>110</v>
+      </c>
+      <c r="I66" s="133"/>
+      <c r="K66" s="167"/>
+    </row>
+    <row r="67" spans="1:11" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="124"/>
+      <c r="B67" s="134" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" s="155"/>
+      <c r="D67" s="165" t="s">
+        <v>72</v>
+      </c>
+      <c r="E67" s="165"/>
+      <c r="F67" s="165"/>
+      <c r="G67" s="165"/>
+      <c r="H67" s="165"/>
+      <c r="I67" s="166"/>
+      <c r="K67" s="167"/>
+    </row>
+    <row r="68" spans="1:11" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="125" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="127" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="151" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" s="127"/>
+      <c r="E68" s="127" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="127" t="s">
+        <v>90</v>
+      </c>
+      <c r="G68" s="127" t="s">
+        <v>90</v>
+      </c>
+      <c r="H68" s="127" t="s">
+        <v>146</v>
+      </c>
+      <c r="I68" s="135" t="s">
+        <v>90</v>
+      </c>
+      <c r="K68" s="167"/>
+    </row>
+    <row r="69" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="125"/>
+      <c r="B69" s="131" t="s">
+        <v>201</v>
+      </c>
+      <c r="C69" s="153"/>
+      <c r="D69" s="163"/>
+      <c r="E69" s="163"/>
+      <c r="F69" s="163"/>
+      <c r="G69" s="163"/>
+      <c r="H69" s="163" t="s">
+        <v>146</v>
+      </c>
+      <c r="I69" s="164"/>
+      <c r="K69" s="167"/>
+    </row>
+    <row r="70" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="125"/>
+      <c r="B70" s="132" t="s">
+        <v>152</v>
+      </c>
+      <c r="C70" s="156"/>
+      <c r="D70" s="132"/>
+      <c r="E70" s="132"/>
+      <c r="F70" s="132"/>
+      <c r="G70" s="132" t="s">
+        <v>86</v>
+      </c>
+      <c r="H70" s="132"/>
+      <c r="I70" s="133" t="s">
+        <v>86</v>
+      </c>
+      <c r="K70" s="167"/>
+    </row>
+    <row r="71" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="125"/>
+      <c r="B71" s="131" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="153"/>
-      <c r="D52" s="92"/>
-      <c r="E52" s="92" t="s">
+      <c r="C71" s="153"/>
+      <c r="D71" s="163"/>
+      <c r="E71" s="163" t="s">
         <v>140</v>
       </c>
-      <c r="F52" s="92" t="s">
+      <c r="F71" s="163" t="s">
         <v>140</v>
       </c>
-      <c r="G52" s="92" t="s">
+      <c r="G71" s="163" t="s">
         <v>140</v>
       </c>
-      <c r="H52" s="92" t="s">
+      <c r="H71" s="163" t="s">
         <v>140</v>
       </c>
-      <c r="I52" s="154" t="s">
+      <c r="I71" s="164" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="102" t="s">
-        <v>178</v>
-      </c>
-      <c r="B53" s="155" t="s">
-        <v>190</v>
-      </c>
-      <c r="C53" s="156" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="155"/>
-      <c r="E53" s="155" t="s">
-        <v>119</v>
-      </c>
-      <c r="F53" s="155" t="s">
-        <v>119</v>
-      </c>
-      <c r="G53" s="155" t="s">
-        <v>119</v>
-      </c>
-      <c r="H53" s="155" t="s">
-        <v>119</v>
-      </c>
-      <c r="I53" s="157" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="102"/>
-      <c r="B54" s="138" t="s">
-        <v>189</v>
-      </c>
-      <c r="C54" s="139" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="140"/>
-      <c r="E54" s="140"/>
-      <c r="F54" s="140"/>
-      <c r="G54" s="140" t="s">
-        <v>119</v>
-      </c>
-      <c r="H54" s="140"/>
-      <c r="I54" s="146" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="102"/>
-      <c r="B55" s="136" t="s">
-        <v>152</v>
-      </c>
-      <c r="C55" s="137" t="s">
-        <v>87</v>
-      </c>
-      <c r="D55" s="136"/>
-      <c r="E55" s="136" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="136" t="s">
-        <v>141</v>
-      </c>
-      <c r="G55" s="136" t="s">
-        <v>141</v>
-      </c>
-      <c r="H55" s="136" t="s">
-        <v>141</v>
-      </c>
-      <c r="I55" s="145" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="102"/>
-      <c r="B56" s="138" t="s">
-        <v>65</v>
-      </c>
-      <c r="C56" s="139"/>
-      <c r="D56" s="140"/>
-      <c r="E56" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="F56" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="G56" s="140"/>
-      <c r="H56" s="140"/>
-      <c r="I56" s="146"/>
-    </row>
-    <row r="57" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="102"/>
-      <c r="B57" s="158" t="s">
-        <v>191</v>
-      </c>
-      <c r="C57" s="159" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="158"/>
-      <c r="E57" s="158" t="s">
-        <v>90</v>
-      </c>
-      <c r="F57" s="158" t="s">
-        <v>90</v>
-      </c>
-      <c r="G57" s="158"/>
-      <c r="H57" s="158"/>
-      <c r="I57" s="160"/>
-    </row>
-    <row r="58" spans="1:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="103" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="213" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="214" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="209"/>
-      <c r="E58" s="209" t="s">
-        <v>143</v>
-      </c>
-      <c r="F58" s="209" t="s">
-        <v>143</v>
-      </c>
-      <c r="G58" s="209"/>
-      <c r="H58" s="209"/>
-      <c r="I58" s="215"/>
-    </row>
-    <row r="59" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="103"/>
-      <c r="B59" s="136" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="D59" s="136"/>
-      <c r="E59" s="136" t="s">
-        <v>144</v>
-      </c>
-      <c r="F59" s="136" t="s">
-        <v>144</v>
-      </c>
-      <c r="G59" s="136" t="s">
-        <v>144</v>
-      </c>
-      <c r="H59" s="136"/>
-      <c r="I59" s="145" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="103"/>
-      <c r="B60" s="138" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="139" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" s="140"/>
-      <c r="E60" s="140" t="s">
-        <v>154</v>
-      </c>
-      <c r="F60" s="140" t="s">
-        <v>154</v>
-      </c>
-      <c r="G60" s="140" t="s">
-        <v>185</v>
-      </c>
-      <c r="H60" s="140" t="s">
-        <v>109</v>
-      </c>
-      <c r="I60" s="146" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="103"/>
-      <c r="B61" s="136" t="s">
-        <v>204</v>
-      </c>
-      <c r="C61" s="137"/>
-      <c r="D61" s="136"/>
-      <c r="E61" s="136"/>
-      <c r="F61" s="136" t="s">
-        <v>2</v>
-      </c>
-      <c r="G61" s="136" t="s">
-        <v>205</v>
-      </c>
-      <c r="H61" s="136" t="s">
-        <v>205</v>
-      </c>
-      <c r="I61" s="145" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="103"/>
-      <c r="B62" s="138" t="s">
-        <v>166</v>
-      </c>
-      <c r="C62" s="139" t="s">
-        <v>163</v>
-      </c>
-      <c r="D62" s="140"/>
-      <c r="E62" s="140"/>
-      <c r="F62" s="140"/>
-      <c r="G62" s="140" t="s">
-        <v>147</v>
-      </c>
-      <c r="H62" s="140"/>
-      <c r="I62" s="146" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="103"/>
-      <c r="B63" s="136" t="s">
-        <v>164</v>
-      </c>
-      <c r="C63" s="137" t="s">
-        <v>163</v>
-      </c>
-      <c r="D63" s="136"/>
-      <c r="E63" s="136"/>
-      <c r="F63" s="136"/>
-      <c r="G63" s="136"/>
-      <c r="H63" s="136"/>
-      <c r="I63" s="145" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="103"/>
-      <c r="B64" s="138" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64" s="139" t="s">
-        <v>21</v>
-      </c>
-      <c r="D64" s="140"/>
-      <c r="E64" s="140"/>
-      <c r="F64" s="140"/>
-      <c r="G64" s="140" t="s">
-        <v>147</v>
-      </c>
-      <c r="H64" s="140"/>
-      <c r="I64" s="146" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="103"/>
-      <c r="B65" s="136" t="s">
-        <v>18</v>
-      </c>
-      <c r="C65" s="137" t="s">
-        <v>20</v>
-      </c>
-      <c r="D65" s="136"/>
-      <c r="E65" s="136"/>
-      <c r="F65" s="136"/>
-      <c r="G65" s="136"/>
-      <c r="H65" s="136" t="s">
-        <v>110</v>
-      </c>
-      <c r="I65" s="145"/>
-    </row>
-    <row r="66" spans="1:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="103"/>
-      <c r="B66" s="148" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="149"/>
-      <c r="D66" s="150" t="s">
-        <v>72</v>
-      </c>
-      <c r="E66" s="150"/>
-      <c r="F66" s="150"/>
-      <c r="G66" s="150"/>
-      <c r="H66" s="150"/>
-      <c r="I66" s="76"/>
-    </row>
-    <row r="67" spans="1:9" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="104" t="s">
-        <v>57</v>
-      </c>
-      <c r="B67" s="155" t="s">
-        <v>191</v>
-      </c>
-      <c r="C67" s="156" t="s">
-        <v>82</v>
-      </c>
-      <c r="D67" s="155"/>
-      <c r="E67" s="155" t="s">
-        <v>90</v>
-      </c>
-      <c r="F67" s="155" t="s">
-        <v>90</v>
-      </c>
-      <c r="G67" s="155" t="s">
-        <v>90</v>
-      </c>
-      <c r="H67" s="155" t="s">
-        <v>146</v>
-      </c>
-      <c r="I67" s="157" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="104"/>
-      <c r="B68" s="138" t="s">
-        <v>201</v>
-      </c>
-      <c r="C68" s="139"/>
-      <c r="D68" s="140"/>
-      <c r="E68" s="140"/>
-      <c r="F68" s="140"/>
-      <c r="G68" s="140"/>
-      <c r="H68" s="140" t="s">
-        <v>146</v>
-      </c>
-      <c r="I68" s="146"/>
-    </row>
-    <row r="69" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="104"/>
-      <c r="B69" s="136" t="s">
-        <v>152</v>
-      </c>
-      <c r="C69" s="137"/>
-      <c r="D69" s="136"/>
-      <c r="E69" s="136"/>
-      <c r="F69" s="136"/>
-      <c r="G69" s="136" t="s">
-        <v>86</v>
-      </c>
-      <c r="H69" s="136"/>
-      <c r="I69" s="145" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="104"/>
-      <c r="B70" s="138" t="s">
-        <v>65</v>
-      </c>
-      <c r="C70" s="139"/>
-      <c r="D70" s="140"/>
-      <c r="E70" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="F70" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="G70" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="H70" s="140" t="s">
-        <v>140</v>
-      </c>
-      <c r="I70" s="146" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="104"/>
-      <c r="B71" s="158" t="s">
+      <c r="K71" s="167"/>
+    </row>
+    <row r="72" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="125"/>
+      <c r="B72" s="136" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="159"/>
-      <c r="D71" s="158"/>
-      <c r="E71" s="158" t="s">
+      <c r="C72" s="154"/>
+      <c r="D72" s="136"/>
+      <c r="E72" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="F71" s="158" t="s">
+      <c r="F72" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="G71" s="158" t="s">
+      <c r="G72" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="H71" s="158"/>
-      <c r="I71" s="160" t="s">
+      <c r="H72" s="136"/>
+      <c r="I72" s="137" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="151" t="s">
+      <c r="K72" s="167"/>
+    </row>
+    <row r="73" spans="1:11" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="152" t="s">
+      <c r="B73" s="130" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="153"/>
-      <c r="D72" s="92" t="s">
+      <c r="C73" s="152"/>
+      <c r="D73" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="E72" s="92"/>
-      <c r="F72" s="92"/>
-      <c r="G72" s="92"/>
-      <c r="H72" s="92"/>
-      <c r="I72" s="154"/>
+      <c r="E73" s="160"/>
+      <c r="F73" s="160"/>
+      <c r="G73" s="160"/>
+      <c r="H73" s="160"/>
+      <c r="I73" s="162"/>
+      <c r="K73" s="167"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H72" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I73" xr:uid="{B76A9991-F60A-4F4E-BE3E-1DD8CE9115F6}"/>
   <mergeCells count="9">
     <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A58:A67"/>
+    <mergeCell ref="A68:A72"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A10:A12"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A22:A50"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="25" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="24" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4092,7 +4127,7 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="101" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -4110,7 +4145,7 @@
       <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="117"/>
+      <c r="A6" s="102"/>
       <c r="B6" s="18"/>
       <c r="C6" s="19"/>
       <c r="D6" s="15"/>
@@ -4120,7 +4155,7 @@
       <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="103" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -4140,7 +4175,7 @@
       <c r="H7" s="64"/>
     </row>
     <row r="8" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="119"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
@@ -4158,7 +4193,7 @@
       <c r="H8" s="67"/>
     </row>
     <row r="9" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="120"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="15" t="s">
         <v>8</v>
       </c>
@@ -4190,7 +4225,7 @@
       <c r="H10" s="69"/>
     </row>
     <row r="11" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="106" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="24" t="s">
@@ -4206,7 +4241,7 @@
       <c r="H11" s="71"/>
     </row>
     <row r="12" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="25" t="s">
         <v>6</v>
       </c>
@@ -4234,7 +4269,7 @@
       <c r="H13" s="69"/>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="101" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="28" t="s">
@@ -4250,7 +4285,7 @@
       <c r="H14" s="71"/>
     </row>
     <row r="15" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="102"/>
       <c r="B15" s="15" t="s">
         <v>6</v>
       </c>
@@ -4266,7 +4301,7 @@
       <c r="H15" s="73"/>
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="123" t="s">
+      <c r="A16" s="108" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -4288,7 +4323,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="124"/>
+      <c r="A17" s="109"/>
       <c r="B17" s="32" t="s">
         <v>51</v>
       </c>
@@ -4310,7 +4345,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="125"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="33" t="s">
         <v>69</v>
       </c>
@@ -4344,7 +4379,7 @@
       <c r="H19" s="78"/>
     </row>
     <row r="20" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="94" t="s">
         <v>53</v>
       </c>
       <c r="B20" s="39" t="s">
@@ -4362,7 +4397,7 @@
       <c r="H20" s="80"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="128"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="35" t="s">
         <v>26</v>
       </c>
@@ -4384,7 +4419,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="128"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="32" t="s">
         <v>27</v>
       </c>
@@ -4400,7 +4435,7 @@
       <c r="H22" s="75"/>
     </row>
     <row r="23" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="128"/>
+      <c r="A23" s="113"/>
       <c r="B23" s="36" t="s">
         <v>89</v>
       </c>
@@ -4420,7 +4455,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="128"/>
+      <c r="A24" s="113"/>
       <c r="B24" s="32" t="s">
         <v>28</v>
       </c>
@@ -4438,7 +4473,7 @@
       <c r="H24" s="75"/>
     </row>
     <row r="25" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="128"/>
+      <c r="A25" s="113"/>
       <c r="B25" s="36" t="s">
         <v>29</v>
       </c>
@@ -4456,7 +4491,7 @@
       <c r="H25" s="75"/>
     </row>
     <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="128"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="32" t="s">
         <v>30</v>
       </c>
@@ -4474,7 +4509,7 @@
       <c r="H26" s="75"/>
     </row>
     <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="128"/>
+      <c r="A27" s="113"/>
       <c r="B27" s="36" t="s">
         <v>31</v>
       </c>
@@ -4492,7 +4527,7 @@
       <c r="H27" s="75"/>
     </row>
     <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="128"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="32" t="s">
         <v>58</v>
       </c>
@@ -4508,7 +4543,7 @@
       <c r="H28" s="75"/>
     </row>
     <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="128"/>
+      <c r="A29" s="113"/>
       <c r="B29" s="36" t="s">
         <v>32</v>
       </c>
@@ -4524,7 +4559,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="128"/>
+      <c r="A30" s="113"/>
       <c r="B30" s="32" t="s">
         <v>91</v>
       </c>
@@ -4540,7 +4575,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="128"/>
+      <c r="A31" s="113"/>
       <c r="B31" s="36" t="s">
         <v>92</v>
       </c>
@@ -4554,7 +4589,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="128"/>
+      <c r="A32" s="113"/>
       <c r="B32" s="32" t="s">
         <v>80</v>
       </c>
@@ -4570,7 +4605,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="128"/>
+      <c r="A33" s="113"/>
       <c r="B33" s="36" t="s">
         <v>33</v>
       </c>
@@ -4586,7 +4621,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="128"/>
+      <c r="A34" s="113"/>
       <c r="B34" s="32" t="s">
         <v>34</v>
       </c>
@@ -4600,7 +4635,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="128"/>
+      <c r="A35" s="113"/>
       <c r="B35" s="36" t="s">
         <v>67</v>
       </c>
@@ -4614,7 +4649,7 @@
       <c r="H35" s="75"/>
     </row>
     <row r="36" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="128"/>
+      <c r="A36" s="113"/>
       <c r="B36" s="37" t="s">
         <v>68</v>
       </c>
@@ -4628,7 +4663,7 @@
       <c r="H36" s="76"/>
     </row>
     <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="128"/>
+      <c r="A37" s="113"/>
       <c r="B37" s="36" t="s">
         <v>159</v>
       </c>
@@ -4646,7 +4681,7 @@
       <c r="H37" s="75"/>
     </row>
     <row r="38" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="110"/>
+      <c r="A38" s="95"/>
       <c r="B38" s="37" t="s">
         <v>161</v>
       </c>
@@ -4682,7 +4717,7 @@
       <c r="H39" s="78"/>
     </row>
     <row r="40" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="126" t="s">
+      <c r="A40" s="111" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="39" t="s">
@@ -4704,7 +4739,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="127"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="33" t="s">
         <v>152</v>
       </c>
@@ -4724,7 +4759,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="109" t="s">
+      <c r="A42" s="94" t="s">
         <v>99</v>
       </c>
       <c r="B42" s="39" t="s">
@@ -4744,7 +4779,7 @@
       <c r="H42" s="84"/>
     </row>
     <row r="43" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="110"/>
+      <c r="A43" s="95"/>
       <c r="B43" s="33" t="s">
         <v>65</v>
       </c>
@@ -4760,7 +4795,7 @@
       <c r="H43" s="86"/>
     </row>
     <row r="44" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="111" t="s">
+      <c r="A44" s="96" t="s">
         <v>56</v>
       </c>
       <c r="B44" s="39" t="s">
@@ -4780,7 +4815,7 @@
       <c r="H44" s="84"/>
     </row>
     <row r="45" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="112"/>
+      <c r="A45" s="97"/>
       <c r="B45" s="36" t="s">
         <v>15</v>
       </c>
@@ -4800,7 +4835,7 @@
       <c r="H45" s="75"/>
     </row>
     <row r="46" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="112"/>
+      <c r="A46" s="97"/>
       <c r="B46" s="32" t="s">
         <v>16</v>
       </c>
@@ -4822,7 +4857,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="112"/>
+      <c r="A47" s="97"/>
       <c r="B47" s="36" t="s">
         <v>84</v>
       </c>
@@ -4838,7 +4873,7 @@
       <c r="H47" s="75"/>
     </row>
     <row r="48" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="112"/>
+      <c r="A48" s="97"/>
       <c r="B48" s="32" t="s">
         <v>18</v>
       </c>
@@ -4854,7 +4889,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="113"/>
+      <c r="A49" s="98"/>
       <c r="B49" s="33" t="s">
         <v>71</v>
       </c>
@@ -4868,7 +4903,7 @@
       <c r="H49" s="86"/>
     </row>
     <row r="50" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="114" t="s">
+      <c r="A50" s="99" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="39" t="s">
@@ -4892,7 +4927,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="114"/>
+      <c r="A51" s="99"/>
       <c r="B51" s="36" t="s">
         <v>152</v>
       </c>
@@ -4906,7 +4941,7 @@
       <c r="H51" s="75"/>
     </row>
     <row r="52" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="114"/>
+      <c r="A52" s="99"/>
       <c r="B52" s="32" t="s">
         <v>65</v>
       </c>
@@ -4926,7 +4961,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="115"/>
+      <c r="A53" s="100"/>
       <c r="B53" s="33" t="s">
         <v>66</v>
       </c>

</xml_diff>